<commit_message>
cierre 29 abr 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #04  ABRIL   2022/BALANCE    ZAVALETA   ABRIL  2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #04  ABRIL   2022/BALANCE    ZAVALETA   ABRIL  2022.xlsx
@@ -541,7 +541,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="651">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -2479,6 +2479,21 @@
   </si>
   <si>
     <t>POLLO-QUESOS-SALCHICHONERIA</t>
+  </si>
+  <si>
+    <t>BALANCE      ABASTO 4 CARNES    Z A V A L E T A      FEBRERO           2 0 2 2</t>
+  </si>
+  <si>
+    <t>QUESOS-ENCHILADA-LONGANIZA</t>
+  </si>
+  <si>
+    <t>QUESO-POLLO-JAMON-ARABE</t>
+  </si>
+  <si>
+    <t>NOMINA # 17  y vacaciones Pedro</t>
+  </si>
+  <si>
+    <t>Nomina # 17 y vacaciones Pedro</t>
   </si>
 </sst>
 </file>
@@ -4285,7 +4300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="613">
+  <cellXfs count="614">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -5298,7 +5313,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="21" borderId="86" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="16" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="94" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -5614,6 +5628,12 @@
     </xf>
     <xf numFmtId="0" fontId="33" fillId="6" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9038,23 +9058,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="509"/>
-      <c r="C1" s="511" t="s">
+      <c r="B1" s="508"/>
+      <c r="C1" s="510" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="512"/>
-      <c r="E1" s="512"/>
-      <c r="F1" s="512"/>
-      <c r="G1" s="512"/>
-      <c r="H1" s="512"/>
-      <c r="I1" s="512"/>
-      <c r="J1" s="512"/>
-      <c r="K1" s="512"/>
-      <c r="L1" s="512"/>
-      <c r="M1" s="512"/>
+      <c r="D1" s="511"/>
+      <c r="E1" s="511"/>
+      <c r="F1" s="511"/>
+      <c r="G1" s="511"/>
+      <c r="H1" s="511"/>
+      <c r="I1" s="511"/>
+      <c r="J1" s="511"/>
+      <c r="K1" s="511"/>
+      <c r="L1" s="511"/>
+      <c r="M1" s="511"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="510"/>
+      <c r="B2" s="509"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -9064,17 +9084,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="513" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="514"/>
+      <c r="B3" s="512" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="513"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="515" t="s">
+      <c r="H3" s="514" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="515"/>
+      <c r="I3" s="514"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -9088,14 +9108,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="516" t="s">
+      <c r="E4" s="515" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="517"/>
-      <c r="H4" s="518" t="s">
+      <c r="F4" s="516"/>
+      <c r="H4" s="517" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="519"/>
+      <c r="I4" s="518"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -9105,10 +9125,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="525" t="s">
+      <c r="P4" s="524" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="526"/>
+      <c r="Q4" s="525"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -10549,11 +10569,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="527">
+      <c r="M39" s="526">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="529">
+      <c r="N39" s="528">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -10579,8 +10599,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="528"/>
-      <c r="N40" s="530"/>
+      <c r="M40" s="527"/>
+      <c r="N40" s="529"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -10795,29 +10815,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="531" t="s">
+      <c r="H52" s="530" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="532"/>
+      <c r="I52" s="531"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="533">
+      <c r="K52" s="532">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="534"/>
-      <c r="M52" s="535">
+      <c r="L52" s="533"/>
+      <c r="M52" s="534">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="536"/>
+      <c r="N52" s="535"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="537" t="s">
+      <c r="D53" s="536" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="537"/>
+      <c r="E53" s="536"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -10828,22 +10848,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="537" t="s">
+      <c r="D54" s="536" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="537"/>
+      <c r="E54" s="536"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="538" t="s">
+      <c r="I54" s="537" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="539"/>
-      <c r="K54" s="540">
+      <c r="J54" s="538"/>
+      <c r="K54" s="539">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="541"/>
+      <c r="L54" s="540"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -10876,11 +10896,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="542">
+      <c r="K56" s="541">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="543"/>
+      <c r="L56" s="542"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -10897,22 +10917,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="520" t="s">
+      <c r="D58" s="519" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="521"/>
+      <c r="E58" s="520"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="522" t="s">
+      <c r="I58" s="521" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="523"/>
-      <c r="K58" s="524">
+      <c r="J58" s="522"/>
+      <c r="K58" s="523">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="524"/>
+      <c r="L58" s="523"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -13536,10 +13556,10 @@
         <f t="shared" si="3"/>
         <v>188840.46999999997</v>
       </c>
-      <c r="I76" s="605" t="s">
+      <c r="I76" s="604" t="s">
         <v>597</v>
       </c>
-      <c r="J76" s="606"/>
+      <c r="J76" s="605"/>
       <c r="K76" s="69"/>
       <c r="L76" s="148"/>
       <c r="M76" s="69"/>
@@ -13558,8 +13578,8 @@
         <f t="shared" si="3"/>
         <v>188840.46999999997</v>
       </c>
-      <c r="I77" s="607"/>
-      <c r="J77" s="608"/>
+      <c r="I77" s="606"/>
+      <c r="J77" s="607"/>
       <c r="K77" s="69"/>
       <c r="L77" s="148"/>
       <c r="M77" s="69"/>
@@ -13626,7 +13646,7 @@
       <c r="C80" s="214"/>
       <c r="D80" s="256"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="571" t="s">
+      <c r="F80" s="570" t="s">
         <v>207</v>
       </c>
       <c r="K80" s="1"/>
@@ -13641,7 +13661,7 @@
       <c r="C81" s="463"/>
       <c r="D81" s="464"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="572"/>
+      <c r="F81" s="571"/>
       <c r="K81" s="1"/>
       <c r="L81" s="97"/>
       <c r="M81" s="3"/>
@@ -13649,10 +13669,10 @@
     </row>
     <row r="82" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A82" s="435"/>
-      <c r="B82" s="604" t="s">
+      <c r="B82" s="603" t="s">
         <v>595</v>
       </c>
-      <c r="C82" s="604"/>
+      <c r="C82" s="603"/>
       <c r="I82"/>
       <c r="J82" s="194"/>
     </row>
@@ -13904,8 +13924,8 @@
   </sheetPr>
   <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13934,23 +13954,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="509"/>
-      <c r="C1" s="575" t="s">
+      <c r="B1" s="508"/>
+      <c r="C1" s="574" t="s">
         <v>451</v>
       </c>
-      <c r="D1" s="576"/>
-      <c r="E1" s="576"/>
-      <c r="F1" s="576"/>
-      <c r="G1" s="576"/>
-      <c r="H1" s="576"/>
-      <c r="I1" s="576"/>
-      <c r="J1" s="576"/>
-      <c r="K1" s="576"/>
-      <c r="L1" s="576"/>
-      <c r="M1" s="576"/>
+      <c r="D1" s="575"/>
+      <c r="E1" s="575"/>
+      <c r="F1" s="575"/>
+      <c r="G1" s="575"/>
+      <c r="H1" s="575"/>
+      <c r="I1" s="575"/>
+      <c r="J1" s="575"/>
+      <c r="K1" s="575"/>
+      <c r="L1" s="575"/>
+      <c r="M1" s="575"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="510"/>
+      <c r="B2" s="509"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -13960,24 +13980,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="513" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="514"/>
+      <c r="B3" s="512" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="513"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="515" t="s">
+      <c r="H3" s="514" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="515"/>
+      <c r="I3" s="514"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="552" t="s">
+      <c r="P3" s="551" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="573" t="s">
+      <c r="R3" s="572" t="s">
         <v>216</v>
       </c>
     </row>
@@ -13992,14 +14012,14 @@
       <c r="D4" s="18">
         <v>44619</v>
       </c>
-      <c r="E4" s="516" t="s">
+      <c r="E4" s="515" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="517"/>
-      <c r="H4" s="518" t="s">
+      <c r="F4" s="516"/>
+      <c r="H4" s="517" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="519"/>
+      <c r="I4" s="518"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -14009,15 +14029,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="553"/>
+      <c r="P4" s="552"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="574"/>
-      <c r="W4" s="562" t="s">
+      <c r="R4" s="573"/>
+      <c r="W4" s="561" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="562"/>
+      <c r="X4" s="561"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -14049,7 +14069,7 @@
       <c r="J5" s="37"/>
       <c r="K5" s="31"/>
       <c r="L5" s="9"/>
-      <c r="M5" s="504">
+      <c r="M5" s="32">
         <v>52267</v>
       </c>
       <c r="N5" s="33">
@@ -14068,8 +14088,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="562"/>
-      <c r="X5" s="562"/>
+      <c r="W5" s="561"/>
+      <c r="X5" s="561"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -14099,7 +14119,7 @@
       <c r="J6" s="37"/>
       <c r="K6" s="38"/>
       <c r="L6" s="39"/>
-      <c r="M6" s="504">
+      <c r="M6" s="32">
         <v>33586.5</v>
       </c>
       <c r="N6" s="33">
@@ -14153,7 +14173,7 @@
       <c r="J7" s="37"/>
       <c r="K7" s="38"/>
       <c r="L7" s="39"/>
-      <c r="M7" s="504">
+      <c r="M7" s="32">
         <v>38157</v>
       </c>
       <c r="N7" s="33">
@@ -14208,7 +14228,7 @@
       <c r="J8" s="43"/>
       <c r="K8" s="38"/>
       <c r="L8" s="39"/>
-      <c r="M8" s="504">
+      <c r="M8" s="32">
         <f>31611+1120</f>
         <v>32731</v>
       </c>
@@ -14265,7 +14285,7 @@
       <c r="J9" s="37"/>
       <c r="K9" s="223"/>
       <c r="L9" s="39"/>
-      <c r="M9" s="504">
+      <c r="M9" s="32">
         <v>57014</v>
       </c>
       <c r="N9" s="33">
@@ -14326,7 +14346,7 @@
       <c r="L10" s="45">
         <v>12109.41</v>
       </c>
-      <c r="M10" s="504">
+      <c r="M10" s="32">
         <v>38720</v>
       </c>
       <c r="N10" s="33">
@@ -14382,7 +14402,7 @@
       <c r="J11" s="43"/>
       <c r="K11" s="168"/>
       <c r="L11" s="39"/>
-      <c r="M11" s="504">
+      <c r="M11" s="32">
         <v>62058</v>
       </c>
       <c r="N11" s="33">
@@ -14438,7 +14458,7 @@
       <c r="J12" s="37"/>
       <c r="K12" s="169"/>
       <c r="L12" s="39"/>
-      <c r="M12" s="504">
+      <c r="M12" s="32">
         <v>20493.5</v>
       </c>
       <c r="N12" s="33">
@@ -14495,7 +14515,7 @@
       <c r="J13" s="37"/>
       <c r="K13" s="38"/>
       <c r="L13" s="39"/>
-      <c r="M13" s="504">
+      <c r="M13" s="32">
         <v>41442.5</v>
       </c>
       <c r="N13" s="33">
@@ -14549,7 +14569,7 @@
       <c r="J14" s="37"/>
       <c r="K14" s="38"/>
       <c r="L14" s="39"/>
-      <c r="M14" s="504">
+      <c r="M14" s="32">
         <f>70135.5+580.16+6869</f>
         <v>77584.66</v>
       </c>
@@ -14602,7 +14622,7 @@
       <c r="J15" s="37"/>
       <c r="K15" s="38"/>
       <c r="L15" s="39"/>
-      <c r="M15" s="504">
+      <c r="M15" s="32">
         <v>47170</v>
       </c>
       <c r="N15" s="33">
@@ -14653,7 +14673,7 @@
       <c r="J16" s="37"/>
       <c r="K16" s="169"/>
       <c r="L16" s="9"/>
-      <c r="M16" s="504">
+      <c r="M16" s="32">
         <v>60292.5</v>
       </c>
       <c r="N16" s="33">
@@ -14711,7 +14731,7 @@
       <c r="L17" s="45">
         <v>18054.02</v>
       </c>
-      <c r="M17" s="504">
+      <c r="M17" s="32">
         <v>55203</v>
       </c>
       <c r="N17" s="33">
@@ -14762,7 +14782,7 @@
       <c r="J18" s="37"/>
       <c r="K18" s="170"/>
       <c r="L18" s="39"/>
-      <c r="M18" s="504">
+      <c r="M18" s="32">
         <v>47814</v>
       </c>
       <c r="N18" s="33">
@@ -14813,7 +14833,7 @@
       <c r="J19" s="37"/>
       <c r="K19" s="46"/>
       <c r="L19" s="47"/>
-      <c r="M19" s="504">
+      <c r="M19" s="32">
         <f>30013+8142</f>
         <v>38155</v>
       </c>
@@ -14832,7 +14852,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="566">
+      <c r="W19" s="565">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -14866,7 +14886,7 @@
       <c r="J20" s="37"/>
       <c r="K20" s="171"/>
       <c r="L20" s="45"/>
-      <c r="M20" s="504">
+      <c r="M20" s="32">
         <v>33949</v>
       </c>
       <c r="N20" s="33">
@@ -14884,7 +14904,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="567"/>
+      <c r="W20" s="566"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -14915,7 +14935,7 @@
       <c r="J21" s="37"/>
       <c r="K21" s="48"/>
       <c r="L21" s="45"/>
-      <c r="M21" s="504">
+      <c r="M21" s="32">
         <v>65434</v>
       </c>
       <c r="N21" s="33">
@@ -14933,8 +14953,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="568"/>
-      <c r="X21" s="568"/>
+      <c r="W21" s="567"/>
+      <c r="X21" s="567"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -14965,7 +14985,7 @@
       <c r="J22" s="37"/>
       <c r="K22" s="31"/>
       <c r="L22" s="49"/>
-      <c r="M22" s="504">
+      <c r="M22" s="32">
         <f>642+62879</f>
         <v>63521</v>
       </c>
@@ -15016,7 +15036,7 @@
       <c r="J23" s="50"/>
       <c r="K23" s="172"/>
       <c r="L23" s="45"/>
-      <c r="M23" s="504">
+      <c r="M23" s="32">
         <v>53950</v>
       </c>
       <c r="N23" s="33">
@@ -15034,8 +15054,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="569"/>
-      <c r="X23" s="569"/>
+      <c r="W23" s="568"/>
+      <c r="X23" s="568"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -15072,7 +15092,7 @@
       <c r="L24" s="52">
         <v>20799.990000000002</v>
       </c>
-      <c r="M24" s="504">
+      <c r="M24" s="32">
         <v>28076</v>
       </c>
       <c r="N24" s="33">
@@ -15090,8 +15110,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="569"/>
-      <c r="X24" s="569"/>
+      <c r="W24" s="568"/>
+      <c r="X24" s="568"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -15122,7 +15142,7 @@
       <c r="J25" s="50"/>
       <c r="K25" s="38"/>
       <c r="L25" s="54"/>
-      <c r="M25" s="504">
+      <c r="M25" s="32">
         <v>47560.5</v>
       </c>
       <c r="N25" s="33">
@@ -15139,8 +15159,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="570"/>
-      <c r="X25" s="570"/>
+      <c r="W25" s="569"/>
+      <c r="X25" s="569"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -15171,7 +15191,7 @@
       <c r="J26" s="37"/>
       <c r="K26" s="173"/>
       <c r="L26" s="45"/>
-      <c r="M26" s="504">
+      <c r="M26" s="32">
         <v>36536</v>
       </c>
       <c r="N26" s="33">
@@ -15189,8 +15209,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="570"/>
-      <c r="X26" s="570"/>
+      <c r="W26" s="569"/>
+      <c r="X26" s="569"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -15221,7 +15241,7 @@
       <c r="J27" s="55"/>
       <c r="K27" s="174"/>
       <c r="L27" s="54"/>
-      <c r="M27" s="504">
+      <c r="M27" s="32">
         <v>42310.5</v>
       </c>
       <c r="N27" s="33">
@@ -15238,9 +15258,9 @@
       <c r="R27" s="388">
         <v>170</v>
       </c>
-      <c r="W27" s="563"/>
-      <c r="X27" s="564"/>
-      <c r="Y27" s="565"/>
+      <c r="W27" s="562"/>
+      <c r="X27" s="563"/>
+      <c r="Y27" s="564"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -15270,7 +15290,7 @@
       <c r="J28" s="56"/>
       <c r="K28" s="57"/>
       <c r="L28" s="54"/>
-      <c r="M28" s="504">
+      <c r="M28" s="32">
         <f>49352+673725.34+200000+33828.02</f>
         <v>956905.36</v>
       </c>
@@ -15288,9 +15308,9 @@
       <c r="R28" s="388">
         <v>37374.36</v>
       </c>
-      <c r="W28" s="564"/>
-      <c r="X28" s="564"/>
-      <c r="Y28" s="565"/>
+      <c r="W28" s="563"/>
+      <c r="X28" s="563"/>
+      <c r="Y28" s="564"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -15320,7 +15340,7 @@
       <c r="J29" s="59"/>
       <c r="K29" s="175"/>
       <c r="L29" s="54"/>
-      <c r="M29" s="504">
+      <c r="M29" s="32">
         <f>642+79978</f>
         <v>80620</v>
       </c>
@@ -15375,7 +15395,7 @@
       <c r="J30" s="60"/>
       <c r="K30" s="41"/>
       <c r="L30" s="61"/>
-      <c r="M30" s="504">
+      <c r="M30" s="32">
         <v>48450</v>
       </c>
       <c r="N30" s="33">
@@ -15432,7 +15452,7 @@
       <c r="L31" s="460">
         <v>19492.72</v>
       </c>
-      <c r="M31" s="504">
+      <c r="M31" s="32">
         <v>28431</v>
       </c>
       <c r="N31" s="33">
@@ -15481,7 +15501,7 @@
       <c r="J32" s="60"/>
       <c r="K32" s="41"/>
       <c r="L32" s="61"/>
-      <c r="M32" s="504">
+      <c r="M32" s="32">
         <v>32180</v>
       </c>
       <c r="N32" s="33">
@@ -15622,11 +15642,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="554">
+      <c r="M36" s="553">
         <f>SUM(M5:M35)</f>
         <v>2220612.02</v>
       </c>
-      <c r="N36" s="556">
+      <c r="N36" s="555">
         <f>SUM(N5:N35)</f>
         <v>833865</v>
       </c>
@@ -15634,7 +15654,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="600">
+      <c r="Q36" s="599">
         <f>SUM(Q5:Q35)</f>
         <v>8.3000000000320142</v>
       </c>
@@ -15659,13 +15679,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="555"/>
-      <c r="N37" s="557"/>
+      <c r="M37" s="554"/>
+      <c r="N37" s="556"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="601"/>
+      <c r="Q37" s="600"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -15710,11 +15730,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="602">
+      <c r="M39" s="601">
         <f>M36+N36</f>
         <v>3054477.02</v>
       </c>
-      <c r="N39" s="603"/>
+      <c r="N39" s="602"/>
       <c r="P39" s="34">
         <f>SUM(P5:P38)</f>
         <v>3627989.66</v>
@@ -15974,26 +15994,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="531" t="s">
+      <c r="H52" s="530" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="532"/>
+      <c r="I52" s="531"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="533">
+      <c r="K52" s="532">
         <f>I50+L50</f>
         <v>217159.4</v>
       </c>
-      <c r="L52" s="560"/>
+      <c r="L52" s="559"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="537" t="s">
+      <c r="D53" s="536" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="537"/>
+      <c r="E53" s="536"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>1453241.94</v>
@@ -16002,22 +16022,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="561" t="s">
+      <c r="D54" s="560" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="561"/>
+      <c r="E54" s="560"/>
       <c r="F54" s="111">
         <v>-1360260.32</v>
       </c>
-      <c r="I54" s="538" t="s">
+      <c r="I54" s="537" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="539"/>
-      <c r="K54" s="540">
+      <c r="J54" s="538"/>
+      <c r="K54" s="539">
         <f>F56+F57+F58</f>
         <v>1797288.1999999997</v>
       </c>
-      <c r="L54" s="540"/>
+      <c r="L54" s="539"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -16058,11 +16078,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="542">
+      <c r="K56" s="541">
         <f>-C4</f>
         <v>-1266568.45</v>
       </c>
-      <c r="L56" s="543"/>
+      <c r="L56" s="542"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -16079,22 +16099,22 @@
       <c r="C58" s="112">
         <v>44647</v>
       </c>
-      <c r="D58" s="520" t="s">
+      <c r="D58" s="519" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="521"/>
+      <c r="E58" s="520"/>
       <c r="F58" s="113">
         <v>1792817.68</v>
       </c>
-      <c r="I58" s="522" t="s">
+      <c r="I58" s="521" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="523"/>
-      <c r="K58" s="524">
+      <c r="J58" s="522"/>
+      <c r="K58" s="523">
         <f>K54+K56</f>
         <v>530719.74999999977</v>
       </c>
-      <c r="L58" s="524"/>
+      <c r="L58" s="523"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -16284,7 +16304,7 @@
   <dimension ref="A1:N115"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A22" sqref="A1:XFD1048576"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18446,7 +18466,7 @@
       <c r="C80" s="214"/>
       <c r="D80" s="256"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="571" t="s">
+      <c r="F80" s="570" t="s">
         <v>207</v>
       </c>
       <c r="K80" s="1"/>
@@ -18459,7 +18479,7 @@
       <c r="C81" s="1"/>
       <c r="D81" s="256"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="572"/>
+      <c r="F81" s="571"/>
       <c r="K81" s="1"/>
       <c r="L81" s="97"/>
       <c r="M81" s="3"/>
@@ -18479,16 +18499,16 @@
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="456"/>
       <c r="B83" s="442"/>
-      <c r="I83" s="609" t="s">
+      <c r="I83" s="608" t="s">
         <v>594</v>
       </c>
-      <c r="J83" s="610"/>
+      <c r="J83" s="609"/>
     </row>
     <row r="84" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="456"/>
       <c r="B84" s="442"/>
-      <c r="I84" s="611"/>
-      <c r="J84" s="612"/>
+      <c r="I84" s="610"/>
+      <c r="J84" s="611"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="456"/>
@@ -18755,8 +18775,8 @@
   </sheetPr>
   <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I16" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -18785,23 +18805,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="509"/>
-      <c r="C1" s="575" t="s">
+      <c r="B1" s="508"/>
+      <c r="C1" s="574" t="s">
         <v>620</v>
       </c>
-      <c r="D1" s="576"/>
-      <c r="E1" s="576"/>
-      <c r="F1" s="576"/>
-      <c r="G1" s="576"/>
-      <c r="H1" s="576"/>
-      <c r="I1" s="576"/>
-      <c r="J1" s="576"/>
-      <c r="K1" s="576"/>
-      <c r="L1" s="576"/>
-      <c r="M1" s="576"/>
+      <c r="D1" s="575"/>
+      <c r="E1" s="575"/>
+      <c r="F1" s="575"/>
+      <c r="G1" s="575"/>
+      <c r="H1" s="575"/>
+      <c r="I1" s="575"/>
+      <c r="J1" s="575"/>
+      <c r="K1" s="575"/>
+      <c r="L1" s="575"/>
+      <c r="M1" s="575"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="510"/>
+      <c r="B2" s="509"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -18811,24 +18831,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="513" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="514"/>
+      <c r="B3" s="512" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="513"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="515" t="s">
+      <c r="H3" s="514" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="515"/>
+      <c r="I3" s="514"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="552" t="s">
+      <c r="P3" s="551" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="573" t="s">
+      <c r="R3" s="572" t="s">
         <v>216</v>
       </c>
     </row>
@@ -18843,14 +18863,14 @@
       <c r="D4" s="18">
         <v>44647</v>
       </c>
-      <c r="E4" s="516" t="s">
+      <c r="E4" s="515" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="517"/>
-      <c r="H4" s="518" t="s">
+      <c r="F4" s="516"/>
+      <c r="H4" s="517" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="519"/>
+      <c r="I4" s="518"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -18860,15 +18880,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="553"/>
+      <c r="P4" s="552"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="574"/>
-      <c r="W4" s="562" t="s">
+      <c r="R4" s="573"/>
+      <c r="W4" s="561" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="562"/>
+      <c r="X4" s="561"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -18919,8 +18939,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="562"/>
-      <c r="X5" s="562"/>
+      <c r="W5" s="561"/>
+      <c r="X5" s="561"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -19679,7 +19699,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="566">
+      <c r="W19" s="565">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -19731,7 +19751,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="567"/>
+      <c r="W20" s="566"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -19780,8 +19800,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="568"/>
-      <c r="X21" s="568"/>
+      <c r="W21" s="567"/>
+      <c r="X21" s="567"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -19878,8 +19898,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="569"/>
-      <c r="X23" s="569"/>
+      <c r="W23" s="568"/>
+      <c r="X23" s="568"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -19934,8 +19954,8 @@
         <v>642</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="569"/>
-      <c r="X24" s="569"/>
+      <c r="W24" s="568"/>
+      <c r="X24" s="568"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -19981,8 +20001,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="570"/>
-      <c r="X25" s="570"/>
+      <c r="W25" s="569"/>
+      <c r="X25" s="569"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -20013,7 +20033,7 @@
       <c r="J26" s="37"/>
       <c r="K26" s="173"/>
       <c r="L26" s="45"/>
-      <c r="M26" s="182">
+      <c r="M26" s="32">
         <f>26691+51054.31+554929.3</f>
         <v>632674.6100000001</v>
       </c>
@@ -20031,8 +20051,8 @@
       <c r="R26" s="388">
         <v>73524.61</v>
       </c>
-      <c r="W26" s="570"/>
-      <c r="X26" s="570"/>
+      <c r="W26" s="569"/>
+      <c r="X26" s="569"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -20063,8 +20083,8 @@
       <c r="J27" s="55"/>
       <c r="K27" s="174"/>
       <c r="L27" s="54"/>
-      <c r="M27" s="182">
-        <v>40223</v>
+      <c r="M27" s="32">
+        <v>39942</v>
       </c>
       <c r="N27" s="33">
         <v>24965</v>
@@ -20072,18 +20092,18 @@
       <c r="O27" s="2"/>
       <c r="P27" s="39">
         <f t="shared" si="1"/>
-        <v>87344</v>
+        <v>87063</v>
       </c>
       <c r="Q27" s="325">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-281</v>
       </c>
       <c r="R27" s="319">
         <v>0</v>
       </c>
-      <c r="W27" s="563"/>
-      <c r="X27" s="564"/>
-      <c r="Y27" s="565"/>
+      <c r="W27" s="562"/>
+      <c r="X27" s="563"/>
+      <c r="Y27" s="564"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -20113,7 +20133,7 @@
       <c r="J28" s="56"/>
       <c r="K28" s="57"/>
       <c r="L28" s="54"/>
-      <c r="M28" s="182">
+      <c r="M28" s="32">
         <v>46851.5</v>
       </c>
       <c r="N28" s="33">
@@ -20131,9 +20151,9 @@
       <c r="R28" s="319">
         <v>0</v>
       </c>
-      <c r="W28" s="564"/>
-      <c r="X28" s="564"/>
-      <c r="Y28" s="565"/>
+      <c r="W28" s="563"/>
+      <c r="X28" s="563"/>
+      <c r="Y28" s="564"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -20163,7 +20183,7 @@
       <c r="J29" s="59"/>
       <c r="K29" s="175"/>
       <c r="L29" s="54"/>
-      <c r="M29" s="182">
+      <c r="M29" s="32">
         <v>55917</v>
       </c>
       <c r="N29" s="33">
@@ -20195,26 +20215,38 @@
       <c r="B30" s="24">
         <v>44673</v>
       </c>
-      <c r="C30" s="25"/>
-      <c r="D30" s="58"/>
+      <c r="C30" s="25">
+        <v>7157</v>
+      </c>
+      <c r="D30" s="58" t="s">
+        <v>647</v>
+      </c>
       <c r="E30" s="27">
         <v>44673</v>
       </c>
-      <c r="F30" s="28"/>
+      <c r="F30" s="28">
+        <v>146405</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="36">
         <v>44673</v>
       </c>
-      <c r="I30" s="30"/>
+      <c r="I30" s="30">
+        <v>3389.5</v>
+      </c>
       <c r="J30" s="60"/>
       <c r="K30" s="41"/>
       <c r="L30" s="61"/>
-      <c r="M30" s="32"/>
-      <c r="N30" s="33"/>
+      <c r="M30" s="32">
+        <v>95058.5</v>
+      </c>
+      <c r="N30" s="33">
+        <v>40800</v>
+      </c>
       <c r="O30" s="426"/>
       <c r="P30" s="34">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>146405</v>
       </c>
       <c r="Q30" s="325">
         <f t="shared" si="0"/>
@@ -20229,35 +20261,50 @@
       <c r="X30" s="225"/>
       <c r="Y30" s="227"/>
     </row>
-    <row r="31" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" ht="26.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="23"/>
       <c r="B31" s="24">
         <v>44674</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="65"/>
+      <c r="C31" s="25">
+        <v>12849.5</v>
+      </c>
+      <c r="D31" s="67" t="s">
+        <v>648</v>
+      </c>
       <c r="E31" s="27">
         <v>44674</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="28">
+        <v>128304</v>
+      </c>
       <c r="G31" s="2"/>
       <c r="H31" s="36">
         <v>44674</v>
       </c>
-      <c r="I31" s="30"/>
-      <c r="J31" s="60"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="63"/>
+      <c r="I31" s="30">
+        <v>4268.5</v>
+      </c>
+      <c r="J31" s="60">
+        <v>44674</v>
+      </c>
+      <c r="K31" s="613" t="s">
+        <v>649</v>
+      </c>
+      <c r="L31" s="63">
+        <f>19296.22+4821.43</f>
+        <v>24117.65</v>
+      </c>
       <c r="M31" s="32"/>
       <c r="N31" s="33"/>
       <c r="O31" s="425"/>
       <c r="P31" s="34">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>41235.65</v>
       </c>
       <c r="Q31" s="325">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-87068.35</v>
       </c>
       <c r="R31" s="319">
         <v>0</v>
@@ -20420,21 +20467,21 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="554">
+      <c r="M36" s="553">
         <f>SUM(M5:M35)</f>
-        <v>1788632.61</v>
-      </c>
-      <c r="N36" s="556">
+        <v>1883410.11</v>
+      </c>
+      <c r="N36" s="555">
         <f>SUM(N5:N35)</f>
-        <v>828721</v>
+        <v>869521</v>
       </c>
       <c r="O36" s="276"/>
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="600">
+      <c r="Q36" s="599">
         <f>SUM(Q5:Q35)</f>
-        <v>284.97999999999593</v>
+        <v>-87064.37000000001</v>
       </c>
       <c r="R36" s="228"/>
     </row>
@@ -20457,13 +20504,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="555"/>
-      <c r="N37" s="557"/>
+      <c r="M37" s="554"/>
+      <c r="N37" s="556"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="601"/>
+      <c r="Q37" s="600"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -20513,14 +20560,14 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="602">
+      <c r="M39" s="601">
         <f>M36+N36</f>
-        <v>2617353.6100000003</v>
-      </c>
-      <c r="N39" s="603"/>
+        <v>2752931.1100000003</v>
+      </c>
+      <c r="N39" s="602"/>
       <c r="P39" s="34">
         <f>SUM(P5:P38)</f>
-        <v>3092058.59</v>
+        <v>3279418.2399999998</v>
       </c>
       <c r="Q39" s="275"/>
     </row>
@@ -20624,9 +20671,16 @@
       <c r="G44" s="2"/>
       <c r="H44" s="76"/>
       <c r="I44" s="77"/>
-      <c r="J44" s="60"/>
-      <c r="K44" s="41"/>
-      <c r="L44" s="61"/>
+      <c r="J44" s="60">
+        <v>44674</v>
+      </c>
+      <c r="K44" s="612" t="s">
+        <v>650</v>
+      </c>
+      <c r="L44" s="61">
+        <f>15598.49+4821.43</f>
+        <v>20419.919999999998</v>
+      </c>
       <c r="M44" s="269"/>
       <c r="N44" s="269"/>
       <c r="P44" s="34"/>
@@ -20729,7 +20783,7 @@
       </c>
       <c r="C50" s="87">
         <f>SUM(C5:C49)</f>
-        <v>344309</v>
+        <v>364315.5</v>
       </c>
       <c r="D50" s="88"/>
       <c r="E50" s="89" t="s">
@@ -20737,7 +20791,7 @@
       </c>
       <c r="F50" s="90">
         <f>SUM(F5:F49)</f>
-        <v>2978758</v>
+        <v>3253467</v>
       </c>
       <c r="G50" s="88"/>
       <c r="H50" s="91" t="s">
@@ -20745,7 +20799,7 @@
       </c>
       <c r="I50" s="92">
         <f>SUM(I5:I49)</f>
-        <v>73212</v>
+        <v>80870</v>
       </c>
       <c r="J50" s="93"/>
       <c r="K50" s="94" t="s">
@@ -20753,7 +20807,7 @@
       </c>
       <c r="L50" s="95">
         <f>SUM(L5:L49)</f>
-        <v>102979.76999999999</v>
+        <v>147517.34000000003</v>
       </c>
       <c r="M50" s="96"/>
       <c r="N50" s="96"/>
@@ -20771,50 +20825,50 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="531" t="s">
+      <c r="H52" s="530" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="532"/>
+      <c r="I52" s="531"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="533">
+      <c r="K52" s="532">
         <f>I50+L50</f>
-        <v>176191.77</v>
-      </c>
-      <c r="L52" s="560"/>
+        <v>228387.34000000003</v>
+      </c>
+      <c r="L52" s="559"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="537" t="s">
+      <c r="D53" s="536" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="537"/>
+      <c r="E53" s="536"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
-        <v>2458257.23</v>
+        <v>2660764.16</v>
       </c>
       <c r="I53" s="102"/>
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="561" t="s">
+      <c r="D54" s="560" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="561"/>
+      <c r="E54" s="560"/>
       <c r="F54" s="111">
         <v>0</v>
       </c>
-      <c r="I54" s="538" t="s">
+      <c r="I54" s="537" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="539"/>
-      <c r="K54" s="540">
+      <c r="J54" s="538"/>
+      <c r="K54" s="539">
         <f>F56+F57+F58</f>
-        <v>2458257.23</v>
-      </c>
-      <c r="L54" s="540"/>
+        <v>2660764.16</v>
+      </c>
+      <c r="L54" s="539"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -20848,18 +20902,18 @@
       </c>
       <c r="F56" s="96">
         <f>SUM(F53:F55)</f>
-        <v>2458257.23</v>
+        <v>2660764.16</v>
       </c>
       <c r="H56" s="23"/>
       <c r="I56" s="108" t="s">
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="542">
+      <c r="K56" s="541">
         <f>-C4</f>
         <v>-1792817.68</v>
       </c>
-      <c r="L56" s="543"/>
+      <c r="L56" s="542"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -20874,22 +20928,22 @@
     </row>
     <row r="58" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C58" s="112"/>
-      <c r="D58" s="520" t="s">
+      <c r="D58" s="519" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="521"/>
+      <c r="E58" s="520"/>
       <c r="F58" s="113">
         <v>0</v>
       </c>
-      <c r="I58" s="522" t="s">
+      <c r="I58" s="521" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="523"/>
-      <c r="K58" s="524">
+      <c r="J58" s="522"/>
+      <c r="K58" s="523">
         <f>K54+K56</f>
-        <v>665439.55000000005</v>
-      </c>
-      <c r="L58" s="524"/>
+        <v>867946.48000000021</v>
+      </c>
+      <c r="L58" s="523"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -21161,7 +21215,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="507"/>
+      <c r="A3" s="506"/>
       <c r="B3" s="438"/>
       <c r="C3" s="410"/>
       <c r="D3" s="411"/>
@@ -21446,7 +21500,7 @@
       <c r="A17" s="454"/>
       <c r="B17" s="246"/>
       <c r="C17" s="111"/>
-      <c r="D17" s="508"/>
+      <c r="D17" s="507"/>
       <c r="E17" s="111"/>
       <c r="F17" s="111">
         <f t="shared" si="0"/>
@@ -21647,7 +21701,7 @@
       <c r="A27" s="454"/>
       <c r="B27" s="246"/>
       <c r="C27" s="111"/>
-      <c r="D27" s="508"/>
+      <c r="D27" s="507"/>
       <c r="E27" s="111"/>
       <c r="F27" s="111">
         <f t="shared" si="0"/>
@@ -22724,7 +22778,7 @@
       <c r="C80" s="214"/>
       <c r="D80" s="256"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="571" t="s">
+      <c r="F80" s="570" t="s">
         <v>207</v>
       </c>
       <c r="K80" s="1"/>
@@ -22737,7 +22791,7 @@
       <c r="C81" s="1"/>
       <c r="D81" s="256"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="572"/>
+      <c r="F81" s="571"/>
       <c r="K81" s="1"/>
       <c r="L81" s="97"/>
       <c r="M81" s="3"/>
@@ -22748,24 +22802,24 @@
       <c r="B82" s="442"/>
       <c r="H82" s="2"/>
       <c r="I82" s="14"/>
-      <c r="J82" s="505"/>
+      <c r="J82" s="504"/>
       <c r="K82" s="6"/>
-      <c r="L82" s="506"/>
+      <c r="L82" s="505"/>
       <c r="M82" s="6"/>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="456"/>
       <c r="B83" s="442"/>
-      <c r="I83" s="609" t="s">
+      <c r="I83" s="608" t="s">
         <v>594</v>
       </c>
-      <c r="J83" s="610"/>
+      <c r="J83" s="609"/>
     </row>
     <row r="84" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="456"/>
       <c r="B84" s="442"/>
-      <c r="I84" s="611"/>
-      <c r="J84" s="612"/>
+      <c r="I84" s="610"/>
+      <c r="J84" s="611"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="456"/>
@@ -24382,7 +24436,7 @@
       <c r="A41" s="140">
         <v>44507</v>
       </c>
-      <c r="B41" s="544" t="s">
+      <c r="B41" s="543" t="s">
         <v>92</v>
       </c>
       <c r="C41" s="190">
@@ -24414,7 +24468,7 @@
       <c r="A42" s="140" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="545"/>
+      <c r="B42" s="544"/>
       <c r="C42" s="143">
         <v>0</v>
       </c>
@@ -26010,23 +26064,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="509"/>
-      <c r="C1" s="511" t="s">
+      <c r="B1" s="508"/>
+      <c r="C1" s="510" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="512"/>
-      <c r="E1" s="512"/>
-      <c r="F1" s="512"/>
-      <c r="G1" s="512"/>
-      <c r="H1" s="512"/>
-      <c r="I1" s="512"/>
-      <c r="J1" s="512"/>
-      <c r="K1" s="512"/>
-      <c r="L1" s="512"/>
-      <c r="M1" s="512"/>
+      <c r="D1" s="511"/>
+      <c r="E1" s="511"/>
+      <c r="F1" s="511"/>
+      <c r="G1" s="511"/>
+      <c r="H1" s="511"/>
+      <c r="I1" s="511"/>
+      <c r="J1" s="511"/>
+      <c r="K1" s="511"/>
+      <c r="L1" s="511"/>
+      <c r="M1" s="511"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="510"/>
+      <c r="B2" s="509"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -26036,21 +26090,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="513" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="514"/>
+      <c r="B3" s="512" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="513"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="515" t="s">
+      <c r="H3" s="514" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="515"/>
+      <c r="I3" s="514"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="552" t="s">
+      <c r="P3" s="551" t="s">
         <v>6</v>
       </c>
     </row>
@@ -26065,14 +26119,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="516" t="s">
+      <c r="E4" s="515" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="517"/>
-      <c r="H4" s="518" t="s">
+      <c r="F4" s="516"/>
+      <c r="H4" s="517" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="519"/>
+      <c r="I4" s="518"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -26082,14 +26136,14 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="553"/>
+      <c r="P4" s="552"/>
       <c r="Q4" s="286" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="562" t="s">
+      <c r="W4" s="561" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="562"/>
+      <c r="X4" s="561"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -26140,8 +26194,8 @@
         <f>20000+7936</f>
         <v>27936</v>
       </c>
-      <c r="W5" s="562"/>
-      <c r="X5" s="562"/>
+      <c r="W5" s="561"/>
+      <c r="X5" s="561"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -26912,7 +26966,7 @@
         <v>26370</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="566">
+      <c r="W19" s="565">
         <f>SUM(W6:W18)</f>
         <v>935136</v>
       </c>
@@ -26964,7 +27018,7 @@
         <v>16395.830000000002</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="567"/>
+      <c r="W20" s="566"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -27013,8 +27067,8 @@
         <v>19188.82</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="568"/>
-      <c r="X21" s="568"/>
+      <c r="W21" s="567"/>
+      <c r="X21" s="567"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -27115,8 +27169,8 @@
         <v>45217.29</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="569"/>
-      <c r="X23" s="569"/>
+      <c r="W23" s="568"/>
+      <c r="X23" s="568"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -27170,8 +27224,8 @@
         <v>23159.17</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="569"/>
-      <c r="X24" s="569"/>
+      <c r="W24" s="568"/>
+      <c r="X24" s="568"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -27217,8 +27271,8 @@
       <c r="R25" s="285">
         <v>28952</v>
       </c>
-      <c r="W25" s="570"/>
-      <c r="X25" s="570"/>
+      <c r="W25" s="569"/>
+      <c r="X25" s="569"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -27269,8 +27323,8 @@
       <c r="R26" s="285">
         <v>21771.5</v>
       </c>
-      <c r="W26" s="570"/>
-      <c r="X26" s="570"/>
+      <c r="W26" s="569"/>
+      <c r="X26" s="569"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -27318,9 +27372,9 @@
       <c r="R27" s="285">
         <v>14637</v>
       </c>
-      <c r="W27" s="563"/>
-      <c r="X27" s="564"/>
-      <c r="Y27" s="565"/>
+      <c r="W27" s="562"/>
+      <c r="X27" s="563"/>
+      <c r="Y27" s="564"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -27370,9 +27424,9 @@
       <c r="R28" s="285">
         <v>0</v>
       </c>
-      <c r="W28" s="564"/>
-      <c r="X28" s="564"/>
-      <c r="Y28" s="565"/>
+      <c r="W28" s="563"/>
+      <c r="X28" s="563"/>
+      <c r="Y28" s="564"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -27707,11 +27761,11 @@
       <c r="L36" s="44">
         <v>5940</v>
       </c>
-      <c r="M36" s="554">
+      <c r="M36" s="553">
         <f>SUM(M5:M35)</f>
         <v>321168.83</v>
       </c>
-      <c r="N36" s="556">
+      <c r="N36" s="555">
         <f>SUM(N5:N35)</f>
         <v>467016</v>
       </c>
@@ -27719,7 +27773,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="558">
+      <c r="Q36" s="557">
         <f>SUM(Q5:Q35)</f>
         <v>-637069.14000000013</v>
       </c>
@@ -27754,13 +27808,13 @@
       <c r="L37" s="61">
         <v>7929.62</v>
       </c>
-      <c r="M37" s="555"/>
-      <c r="N37" s="557"/>
+      <c r="M37" s="554"/>
+      <c r="N37" s="556"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="559"/>
+      <c r="Q37" s="558"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -28050,26 +28104,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="531" t="s">
+      <c r="H52" s="530" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="532"/>
+      <c r="I52" s="531"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="533">
+      <c r="K52" s="532">
         <f>I50+L50</f>
         <v>71911.59</v>
       </c>
-      <c r="L52" s="560"/>
+      <c r="L52" s="559"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="537" t="s">
+      <c r="D53" s="536" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="537"/>
+      <c r="E53" s="536"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>-25952.549999999814</v>
@@ -28078,29 +28132,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="561" t="s">
+      <c r="D54" s="560" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="561"/>
+      <c r="E54" s="560"/>
       <c r="F54" s="111">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="538" t="s">
+      <c r="I54" s="537" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="539"/>
-      <c r="K54" s="540">
+      <c r="J54" s="538"/>
+      <c r="K54" s="539">
         <f>F56+F57+F58</f>
         <v>1308778.3500000003</v>
       </c>
-      <c r="L54" s="540"/>
-      <c r="M54" s="546" t="s">
+      <c r="L54" s="539"/>
+      <c r="M54" s="545" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="547"/>
-      <c r="O54" s="547"/>
-      <c r="P54" s="547"/>
-      <c r="Q54" s="548"/>
+      <c r="N54" s="546"/>
+      <c r="O54" s="546"/>
+      <c r="P54" s="546"/>
+      <c r="Q54" s="547"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="313" t="s">
@@ -28114,11 +28168,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="549"/>
-      <c r="N55" s="550"/>
-      <c r="O55" s="550"/>
-      <c r="P55" s="550"/>
-      <c r="Q55" s="551"/>
+      <c r="M55" s="548"/>
+      <c r="N55" s="549"/>
+      <c r="O55" s="549"/>
+      <c r="P55" s="549"/>
+      <c r="Q55" s="550"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -28136,11 +28190,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="542">
+      <c r="K56" s="541">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="543"/>
+      <c r="L56" s="542"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -28157,22 +28211,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="520" t="s">
+      <c r="D58" s="519" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="521"/>
+      <c r="E58" s="520"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="522" t="s">
+      <c r="I58" s="521" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="523"/>
-      <c r="K58" s="524">
+      <c r="J58" s="522"/>
+      <c r="K58" s="523">
         <f>K54+K56</f>
         <v>741389.00000000035</v>
       </c>
-      <c r="L58" s="524"/>
+      <c r="L58" s="523"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -30762,7 +30816,7 @@
       <c r="C87" s="214"/>
       <c r="D87" s="97"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="571" t="s">
+      <c r="F87" s="570" t="s">
         <v>207</v>
       </c>
       <c r="K87" s="1"/>
@@ -30775,7 +30829,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="97"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="572"/>
+      <c r="F88" s="571"/>
       <c r="K88" s="1"/>
       <c r="L88" s="256"/>
       <c r="M88" s="3"/>
@@ -31087,23 +31141,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="509"/>
-      <c r="C1" s="511" t="s">
+      <c r="B1" s="508"/>
+      <c r="C1" s="510" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="512"/>
-      <c r="E1" s="512"/>
-      <c r="F1" s="512"/>
-      <c r="G1" s="512"/>
-      <c r="H1" s="512"/>
-      <c r="I1" s="512"/>
-      <c r="J1" s="512"/>
-      <c r="K1" s="512"/>
-      <c r="L1" s="512"/>
-      <c r="M1" s="512"/>
+      <c r="D1" s="511"/>
+      <c r="E1" s="511"/>
+      <c r="F1" s="511"/>
+      <c r="G1" s="511"/>
+      <c r="H1" s="511"/>
+      <c r="I1" s="511"/>
+      <c r="J1" s="511"/>
+      <c r="K1" s="511"/>
+      <c r="L1" s="511"/>
+      <c r="M1" s="511"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="510"/>
+      <c r="B2" s="509"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -31113,24 +31167,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="513" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="514"/>
+      <c r="B3" s="512" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="513"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="515" t="s">
+      <c r="H3" s="514" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="515"/>
+      <c r="I3" s="514"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="552" t="s">
+      <c r="P3" s="551" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="573" t="s">
+      <c r="R3" s="572" t="s">
         <v>216</v>
       </c>
     </row>
@@ -31145,14 +31199,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="516" t="s">
+      <c r="E4" s="515" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="517"/>
-      <c r="H4" s="518" t="s">
+      <c r="F4" s="516"/>
+      <c r="H4" s="517" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="519"/>
+      <c r="I4" s="518"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -31162,15 +31216,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="553"/>
+      <c r="P4" s="552"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="574"/>
-      <c r="W4" s="562" t="s">
+      <c r="R4" s="573"/>
+      <c r="W4" s="561" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="562"/>
+      <c r="X4" s="561"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -31231,8 +31285,8 @@
       <c r="S5" s="324" t="s">
         <v>213</v>
       </c>
-      <c r="W5" s="562"/>
-      <c r="X5" s="562"/>
+      <c r="W5" s="561"/>
+      <c r="X5" s="561"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -31989,7 +32043,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="566">
+      <c r="W19" s="565">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -32041,7 +32095,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="567"/>
+      <c r="W20" s="566"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -32090,8 +32144,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="568"/>
-      <c r="X21" s="568"/>
+      <c r="W21" s="567"/>
+      <c r="X21" s="567"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -32192,8 +32246,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="569"/>
-      <c r="X23" s="569"/>
+      <c r="W23" s="568"/>
+      <c r="X23" s="568"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -32244,8 +32298,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="569"/>
-      <c r="X24" s="569"/>
+      <c r="W24" s="568"/>
+      <c r="X24" s="568"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -32291,8 +32345,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="570"/>
-      <c r="X25" s="570"/>
+      <c r="W25" s="569"/>
+      <c r="X25" s="569"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -32340,8 +32394,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="570"/>
-      <c r="X26" s="570"/>
+      <c r="W26" s="569"/>
+      <c r="X26" s="569"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -32401,9 +32455,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="563"/>
-      <c r="X27" s="564"/>
-      <c r="Y27" s="565"/>
+      <c r="W27" s="562"/>
+      <c r="X27" s="563"/>
+      <c r="Y27" s="564"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -32457,9 +32511,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="564"/>
-      <c r="X28" s="564"/>
-      <c r="Y28" s="565"/>
+      <c r="W28" s="563"/>
+      <c r="X28" s="563"/>
+      <c r="Y28" s="564"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -32775,11 +32829,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="554">
+      <c r="M36" s="553">
         <f>SUM(M5:M35)</f>
         <v>1077791.3</v>
       </c>
-      <c r="N36" s="556">
+      <c r="N36" s="555">
         <f>SUM(N5:N35)</f>
         <v>936398</v>
       </c>
@@ -32787,7 +32841,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="558">
+      <c r="Q36" s="557">
         <f>SUM(Q5:Q35)</f>
         <v>-14262.940000000002</v>
       </c>
@@ -32806,13 +32860,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="555"/>
-      <c r="N37" s="557"/>
+      <c r="M37" s="554"/>
+      <c r="N37" s="556"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="559"/>
+      <c r="Q37" s="558"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -33086,26 +33140,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="531" t="s">
+      <c r="H52" s="530" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="532"/>
+      <c r="I52" s="531"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="533">
+      <c r="K52" s="532">
         <f>I50+L50</f>
         <v>90750.75</v>
       </c>
-      <c r="L52" s="560"/>
+      <c r="L52" s="559"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="537" t="s">
+      <c r="D53" s="536" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="537"/>
+      <c r="E53" s="536"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>1739855.03</v>
@@ -33114,29 +33168,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="561" t="s">
+      <c r="D54" s="560" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="561"/>
+      <c r="E54" s="560"/>
       <c r="F54" s="111">
         <v>-1567070.66</v>
       </c>
-      <c r="I54" s="538" t="s">
+      <c r="I54" s="537" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="539"/>
-      <c r="K54" s="540">
+      <c r="J54" s="538"/>
+      <c r="K54" s="539">
         <f>F56+F57+F58</f>
         <v>703192.8600000001</v>
       </c>
-      <c r="L54" s="540"/>
-      <c r="M54" s="546" t="s">
+      <c r="L54" s="539"/>
+      <c r="M54" s="545" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="547"/>
-      <c r="O54" s="547"/>
-      <c r="P54" s="547"/>
-      <c r="Q54" s="548"/>
+      <c r="N54" s="546"/>
+      <c r="O54" s="546"/>
+      <c r="P54" s="546"/>
+      <c r="Q54" s="547"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="313" t="s">
@@ -33150,11 +33204,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="549"/>
-      <c r="N55" s="550"/>
-      <c r="O55" s="550"/>
-      <c r="P55" s="550"/>
-      <c r="Q55" s="551"/>
+      <c r="M55" s="548"/>
+      <c r="N55" s="549"/>
+      <c r="O55" s="549"/>
+      <c r="P55" s="549"/>
+      <c r="Q55" s="550"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -33172,11 +33226,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="542">
+      <c r="K56" s="541">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="543"/>
+      <c r="L56" s="542"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -33193,22 +33247,22 @@
       <c r="C58" s="112">
         <v>44563</v>
       </c>
-      <c r="D58" s="520" t="s">
+      <c r="D58" s="519" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="521"/>
+      <c r="E58" s="520"/>
       <c r="F58" s="113">
         <v>754143.23</v>
       </c>
-      <c r="I58" s="522" t="s">
+      <c r="I58" s="521" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="523"/>
-      <c r="K58" s="524">
+      <c r="J58" s="522"/>
+      <c r="K58" s="523">
         <f>K54+K56</f>
         <v>135803.51000000013</v>
       </c>
-      <c r="L58" s="524"/>
+      <c r="L58" s="523"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -35771,7 +35825,7 @@
       <c r="C75" s="214"/>
       <c r="D75" s="256"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="571" t="s">
+      <c r="F75" s="570" t="s">
         <v>207</v>
       </c>
       <c r="K75" s="1"/>
@@ -35784,7 +35838,7 @@
       <c r="C76" s="1"/>
       <c r="D76" s="256"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="572"/>
+      <c r="F76" s="571"/>
       <c r="K76" s="1"/>
       <c r="L76" s="256"/>
       <c r="M76" s="3"/>
@@ -36046,7 +36100,7 @@
   </sheetPr>
   <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
@@ -36076,23 +36130,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="509"/>
-      <c r="C1" s="575" t="s">
+      <c r="B1" s="508"/>
+      <c r="C1" s="574" t="s">
         <v>316</v>
       </c>
-      <c r="D1" s="576"/>
-      <c r="E1" s="576"/>
-      <c r="F1" s="576"/>
-      <c r="G1" s="576"/>
-      <c r="H1" s="576"/>
-      <c r="I1" s="576"/>
-      <c r="J1" s="576"/>
-      <c r="K1" s="576"/>
-      <c r="L1" s="576"/>
-      <c r="M1" s="576"/>
+      <c r="D1" s="575"/>
+      <c r="E1" s="575"/>
+      <c r="F1" s="575"/>
+      <c r="G1" s="575"/>
+      <c r="H1" s="575"/>
+      <c r="I1" s="575"/>
+      <c r="J1" s="575"/>
+      <c r="K1" s="575"/>
+      <c r="L1" s="575"/>
+      <c r="M1" s="575"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="510"/>
+      <c r="B2" s="509"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -36102,24 +36156,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="513" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="514"/>
+      <c r="B3" s="512" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="513"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="515" t="s">
+      <c r="H3" s="514" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="515"/>
+      <c r="I3" s="514"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="552" t="s">
+      <c r="P3" s="551" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="573" t="s">
+      <c r="R3" s="572" t="s">
         <v>216</v>
       </c>
     </row>
@@ -36134,14 +36188,14 @@
       <c r="D4" s="18">
         <v>44563</v>
       </c>
-      <c r="E4" s="516" t="s">
+      <c r="E4" s="515" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="517"/>
-      <c r="H4" s="518" t="s">
+      <c r="F4" s="516"/>
+      <c r="H4" s="517" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="519"/>
+      <c r="I4" s="518"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -36151,15 +36205,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="553"/>
+      <c r="P4" s="552"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="574"/>
-      <c r="W4" s="562" t="s">
+      <c r="R4" s="573"/>
+      <c r="W4" s="561" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="562"/>
+      <c r="X4" s="561"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -36210,8 +36264,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="562"/>
-      <c r="X5" s="562"/>
+      <c r="W5" s="561"/>
+      <c r="X5" s="561"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -36975,7 +37029,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="566">
+      <c r="W19" s="565">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -37028,7 +37082,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="567"/>
+      <c r="W20" s="566"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -37077,8 +37131,8 @@
         <v>377273.87</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="568"/>
-      <c r="X21" s="568"/>
+      <c r="W21" s="567"/>
+      <c r="X21" s="567"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -37178,8 +37232,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="569"/>
-      <c r="X23" s="569"/>
+      <c r="W23" s="568"/>
+      <c r="X23" s="568"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -37234,8 +37288,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="569"/>
-      <c r="X24" s="569"/>
+      <c r="W24" s="568"/>
+      <c r="X24" s="568"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -37280,8 +37334,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="570"/>
-      <c r="X25" s="570"/>
+      <c r="W25" s="569"/>
+      <c r="X25" s="569"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -37329,8 +37383,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="570"/>
-      <c r="X26" s="570"/>
+      <c r="W26" s="569"/>
+      <c r="X26" s="569"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -37384,9 +37438,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="563"/>
-      <c r="X27" s="564"/>
-      <c r="Y27" s="565"/>
+      <c r="W27" s="562"/>
+      <c r="X27" s="563"/>
+      <c r="Y27" s="564"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -37440,9 +37494,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="564"/>
-      <c r="X28" s="564"/>
-      <c r="Y28" s="565"/>
+      <c r="W28" s="563"/>
+      <c r="X28" s="563"/>
+      <c r="Y28" s="564"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -37753,11 +37807,11 @@
       <c r="L36" s="44">
         <v>13275.84</v>
       </c>
-      <c r="M36" s="554">
+      <c r="M36" s="553">
         <f>SUM(M5:M35)</f>
         <v>1818445.73</v>
       </c>
-      <c r="N36" s="556">
+      <c r="N36" s="555">
         <f>SUM(N5:N35)</f>
         <v>739014</v>
       </c>
@@ -37765,7 +37819,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="558">
+      <c r="Q36" s="557">
         <f>SUM(Q5:Q35)</f>
         <v>-7.2800000000133878</v>
       </c>
@@ -37790,13 +37844,13 @@
       <c r="L37" s="61">
         <v>15060.32</v>
       </c>
-      <c r="M37" s="555"/>
-      <c r="N37" s="557"/>
+      <c r="M37" s="554"/>
+      <c r="N37" s="556"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="559"/>
+      <c r="Q37" s="558"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -38089,26 +38143,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="531" t="s">
+      <c r="H52" s="530" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="532"/>
+      <c r="I52" s="531"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="533">
+      <c r="K52" s="532">
         <f>I50+L50</f>
         <v>158798.12</v>
       </c>
-      <c r="L52" s="560"/>
+      <c r="L52" s="559"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="537" t="s">
+      <c r="D53" s="536" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="537"/>
+      <c r="E53" s="536"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>2078470.75</v>
@@ -38117,22 +38171,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="561" t="s">
+      <c r="D54" s="560" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="561"/>
+      <c r="E54" s="560"/>
       <c r="F54" s="111">
         <v>-1448401.2</v>
       </c>
-      <c r="I54" s="538" t="s">
+      <c r="I54" s="537" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="539"/>
-      <c r="K54" s="540">
+      <c r="J54" s="538"/>
+      <c r="K54" s="539">
         <f>F56+F57+F58</f>
         <v>1025960.7</v>
       </c>
-      <c r="L54" s="540"/>
+      <c r="L54" s="539"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -38173,11 +38227,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="542">
+      <c r="K56" s="541">
         <f>-C4</f>
         <v>-754143.23</v>
       </c>
-      <c r="L56" s="543"/>
+      <c r="L56" s="542"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -38194,22 +38248,22 @@
       <c r="C58" s="112">
         <v>44591</v>
       </c>
-      <c r="D58" s="520" t="s">
+      <c r="D58" s="519" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="521"/>
+      <c r="E58" s="520"/>
       <c r="F58" s="113">
         <v>1149740.4099999999</v>
       </c>
-      <c r="I58" s="522" t="s">
+      <c r="I58" s="521" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="523"/>
-      <c r="K58" s="524">
+      <c r="J58" s="522"/>
+      <c r="K58" s="523">
         <f>K54+K56</f>
         <v>271817.46999999997</v>
       </c>
-      <c r="L58" s="524"/>
+      <c r="L58" s="523"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -40078,12 +40132,12 @@
     </row>
     <row r="43" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="245"/>
-      <c r="B43" s="577" t="s">
+      <c r="B43" s="576" t="s">
         <v>413</v>
       </c>
-      <c r="C43" s="578"/>
-      <c r="D43" s="578"/>
-      <c r="E43" s="579"/>
+      <c r="C43" s="577"/>
+      <c r="D43" s="577"/>
+      <c r="E43" s="578"/>
       <c r="F43" s="392">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -40111,10 +40165,10 @@
     </row>
     <row r="44" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="245"/>
-      <c r="B44" s="580"/>
-      <c r="C44" s="581"/>
-      <c r="D44" s="581"/>
-      <c r="E44" s="582"/>
+      <c r="B44" s="579"/>
+      <c r="C44" s="580"/>
+      <c r="D44" s="580"/>
+      <c r="E44" s="581"/>
       <c r="F44" s="392">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -40142,10 +40196,10 @@
     </row>
     <row r="45" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="245"/>
-      <c r="B45" s="583"/>
-      <c r="C45" s="584"/>
-      <c r="D45" s="584"/>
-      <c r="E45" s="585"/>
+      <c r="B45" s="582"/>
+      <c r="C45" s="583"/>
+      <c r="D45" s="583"/>
+      <c r="E45" s="584"/>
       <c r="F45" s="392">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -40188,10 +40242,10 @@
     </row>
     <row r="47" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="245"/>
-      <c r="B47" s="592" t="s">
+      <c r="B47" s="591" t="s">
         <v>593</v>
       </c>
-      <c r="C47" s="593"/>
+      <c r="C47" s="592"/>
       <c r="D47" s="253"/>
       <c r="E47" s="69"/>
       <c r="F47" s="137">
@@ -40213,8 +40267,8 @@
     </row>
     <row r="48" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="245"/>
-      <c r="B48" s="594"/>
-      <c r="C48" s="595"/>
+      <c r="B48" s="593"/>
+      <c r="C48" s="594"/>
       <c r="D48" s="253"/>
       <c r="E48" s="69"/>
       <c r="F48" s="137">
@@ -40222,11 +40276,11 @@
         <v>0</v>
       </c>
       <c r="I48" s="348"/>
-      <c r="J48" s="586" t="s">
+      <c r="J48" s="585" t="s">
         <v>414</v>
       </c>
-      <c r="K48" s="587"/>
-      <c r="L48" s="588"/>
+      <c r="K48" s="586"/>
+      <c r="L48" s="587"/>
       <c r="M48" s="206"/>
       <c r="N48" s="137">
         <f>N47+K48-M48</f>
@@ -40244,9 +40298,9 @@
         <v>0</v>
       </c>
       <c r="I49" s="348"/>
-      <c r="J49" s="589"/>
-      <c r="K49" s="590"/>
-      <c r="L49" s="591"/>
+      <c r="J49" s="588"/>
+      <c r="K49" s="589"/>
+      <c r="L49" s="590"/>
       <c r="M49" s="206"/>
       <c r="N49" s="137">
         <f t="shared" si="1"/>
@@ -40263,10 +40317,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I50" s="596" t="s">
+      <c r="I50" s="595" t="s">
         <v>594</v>
       </c>
-      <c r="J50" s="597"/>
+      <c r="J50" s="596"/>
       <c r="K50" s="215">
         <v>0</v>
       </c>
@@ -40287,8 +40341,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I51" s="596"/>
-      <c r="J51" s="597"/>
+      <c r="I51" s="595"/>
+      <c r="J51" s="596"/>
       <c r="K51" s="69"/>
       <c r="L51" s="253"/>
       <c r="M51" s="69"/>
@@ -40307,8 +40361,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I52" s="596"/>
-      <c r="J52" s="597"/>
+      <c r="I52" s="595"/>
+      <c r="J52" s="596"/>
       <c r="K52" s="69"/>
       <c r="L52" s="253"/>
       <c r="M52" s="69"/>
@@ -40327,8 +40381,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I53" s="596"/>
-      <c r="J53" s="597"/>
+      <c r="I53" s="595"/>
+      <c r="J53" s="596"/>
       <c r="K53" s="69"/>
       <c r="L53" s="253"/>
       <c r="M53" s="69"/>
@@ -40347,8 +40401,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I54" s="596"/>
-      <c r="J54" s="597"/>
+      <c r="I54" s="595"/>
+      <c r="J54" s="596"/>
       <c r="K54" s="69"/>
       <c r="L54" s="253"/>
       <c r="M54" s="69"/>
@@ -40367,8 +40421,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I55" s="596"/>
-      <c r="J55" s="597"/>
+      <c r="I55" s="595"/>
+      <c r="J55" s="596"/>
       <c r="K55" s="69"/>
       <c r="L55" s="253"/>
       <c r="M55" s="69"/>
@@ -40387,8 +40441,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I56" s="596"/>
-      <c r="J56" s="597"/>
+      <c r="I56" s="595"/>
+      <c r="J56" s="596"/>
       <c r="K56" s="69"/>
       <c r="L56" s="253"/>
       <c r="M56" s="69"/>
@@ -40407,8 +40461,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I57" s="596"/>
-      <c r="J57" s="597"/>
+      <c r="I57" s="595"/>
+      <c r="J57" s="596"/>
       <c r="K57" s="69"/>
       <c r="L57" s="253"/>
       <c r="M57" s="69"/>
@@ -40427,8 +40481,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I58" s="596"/>
-      <c r="J58" s="597"/>
+      <c r="I58" s="595"/>
+      <c r="J58" s="596"/>
       <c r="K58" s="69"/>
       <c r="L58" s="253"/>
       <c r="M58" s="69"/>
@@ -40447,8 +40501,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I59" s="596"/>
-      <c r="J59" s="597"/>
+      <c r="I59" s="595"/>
+      <c r="J59" s="596"/>
       <c r="K59" s="69"/>
       <c r="L59" s="253"/>
       <c r="M59" s="69"/>
@@ -40467,8 +40521,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I60" s="596"/>
-      <c r="J60" s="597"/>
+      <c r="I60" s="595"/>
+      <c r="J60" s="596"/>
       <c r="K60" s="69"/>
       <c r="L60" s="253"/>
       <c r="M60" s="69"/>
@@ -40487,8 +40541,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I61" s="596"/>
-      <c r="J61" s="597"/>
+      <c r="I61" s="595"/>
+      <c r="J61" s="596"/>
       <c r="K61" s="69"/>
       <c r="L61" s="253"/>
       <c r="M61" s="69"/>
@@ -40507,8 +40561,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I62" s="596"/>
-      <c r="J62" s="597"/>
+      <c r="I62" s="595"/>
+      <c r="J62" s="596"/>
       <c r="K62" s="34"/>
       <c r="L62" s="118"/>
       <c r="M62" s="34"/>
@@ -40527,8 +40581,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I63" s="596"/>
-      <c r="J63" s="597"/>
+      <c r="I63" s="595"/>
+      <c r="J63" s="596"/>
       <c r="K63" s="34"/>
       <c r="L63" s="118"/>
       <c r="M63" s="34"/>
@@ -40547,8 +40601,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I64" s="596"/>
-      <c r="J64" s="597"/>
+      <c r="I64" s="595"/>
+      <c r="J64" s="596"/>
       <c r="K64" s="34"/>
       <c r="L64" s="118"/>
       <c r="M64" s="34"/>
@@ -40567,8 +40621,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I65" s="596"/>
-      <c r="J65" s="597"/>
+      <c r="I65" s="595"/>
+      <c r="J65" s="596"/>
       <c r="K65" s="34"/>
       <c r="L65" s="118"/>
       <c r="M65" s="34"/>
@@ -40587,8 +40641,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I66" s="596"/>
-      <c r="J66" s="597"/>
+      <c r="I66" s="595"/>
+      <c r="J66" s="596"/>
       <c r="K66" s="34"/>
       <c r="L66" s="118"/>
       <c r="M66" s="34"/>
@@ -40607,8 +40661,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I67" s="596"/>
-      <c r="J67" s="597"/>
+      <c r="I67" s="595"/>
+      <c r="J67" s="596"/>
       <c r="K67" s="34"/>
       <c r="L67" s="118"/>
       <c r="M67" s="34"/>
@@ -40627,8 +40681,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I68" s="596"/>
-      <c r="J68" s="597"/>
+      <c r="I68" s="595"/>
+      <c r="J68" s="596"/>
       <c r="K68" s="69"/>
       <c r="L68" s="254"/>
       <c r="M68" s="69"/>
@@ -40647,8 +40701,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I69" s="596"/>
-      <c r="J69" s="597"/>
+      <c r="I69" s="595"/>
+      <c r="J69" s="596"/>
       <c r="K69" s="69"/>
       <c r="L69" s="254"/>
       <c r="M69" s="69"/>
@@ -40667,8 +40721,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I70" s="596"/>
-      <c r="J70" s="597"/>
+      <c r="I70" s="595"/>
+      <c r="J70" s="596"/>
       <c r="K70" s="69"/>
       <c r="L70" s="254"/>
       <c r="M70" s="69"/>
@@ -40687,8 +40741,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I71" s="596"/>
-      <c r="J71" s="597"/>
+      <c r="I71" s="595"/>
+      <c r="J71" s="596"/>
       <c r="K71" s="69"/>
       <c r="L71" s="254"/>
       <c r="M71" s="69"/>
@@ -40707,8 +40761,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I72" s="596"/>
-      <c r="J72" s="597"/>
+      <c r="I72" s="595"/>
+      <c r="J72" s="596"/>
       <c r="K72" s="69"/>
       <c r="L72" s="254"/>
       <c r="M72" s="69"/>
@@ -40727,8 +40781,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I73" s="596"/>
-      <c r="J73" s="597"/>
+      <c r="I73" s="595"/>
+      <c r="J73" s="596"/>
       <c r="K73" s="69"/>
       <c r="L73" s="254"/>
       <c r="M73" s="69"/>
@@ -40747,8 +40801,8 @@
         <f>F73+C74-E74</f>
         <v>0</v>
       </c>
-      <c r="I74" s="596"/>
-      <c r="J74" s="597"/>
+      <c r="I74" s="595"/>
+      <c r="J74" s="596"/>
       <c r="K74" s="69"/>
       <c r="L74" s="254"/>
       <c r="M74" s="69"/>
@@ -40767,8 +40821,8 @@
         <f>F74+C75-E75</f>
         <v>0</v>
       </c>
-      <c r="I75" s="596"/>
-      <c r="J75" s="597"/>
+      <c r="I75" s="595"/>
+      <c r="J75" s="596"/>
       <c r="K75" s="69"/>
       <c r="L75" s="254"/>
       <c r="M75" s="69"/>
@@ -40787,8 +40841,8 @@
         <f>F75+C76-E76</f>
         <v>0</v>
       </c>
-      <c r="I76" s="596"/>
-      <c r="J76" s="597"/>
+      <c r="I76" s="595"/>
+      <c r="J76" s="596"/>
       <c r="K76" s="69"/>
       <c r="L76" s="254"/>
       <c r="M76" s="69"/>
@@ -40807,8 +40861,8 @@
         <f>F76+C77-E77</f>
         <v>0</v>
       </c>
-      <c r="I77" s="596"/>
-      <c r="J77" s="597"/>
+      <c r="I77" s="595"/>
+      <c r="J77" s="596"/>
       <c r="K77" s="69"/>
       <c r="L77" s="254"/>
       <c r="M77" s="69"/>
@@ -40829,8 +40883,8 @@
         <f>F77+C78-E78</f>
         <v>0</v>
       </c>
-      <c r="I78" s="598"/>
-      <c r="J78" s="599"/>
+      <c r="I78" s="597"/>
+      <c r="J78" s="598"/>
       <c r="K78" s="151">
         <v>0</v>
       </c>
@@ -40875,7 +40929,7 @@
       <c r="C80" s="214"/>
       <c r="D80" s="256"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="571" t="s">
+      <c r="F80" s="570" t="s">
         <v>207</v>
       </c>
       <c r="K80" s="1"/>
@@ -40887,7 +40941,7 @@
       <c r="C81" s="1"/>
       <c r="D81" s="256"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="572"/>
+      <c r="F81" s="571"/>
       <c r="K81" s="1"/>
       <c r="M81" s="3"/>
       <c r="N81" s="1"/>
@@ -41145,8 +41199,8 @@
   </sheetPr>
   <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -41175,23 +41229,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="509"/>
-      <c r="C1" s="575" t="s">
-        <v>316</v>
-      </c>
-      <c r="D1" s="576"/>
-      <c r="E1" s="576"/>
-      <c r="F1" s="576"/>
-      <c r="G1" s="576"/>
-      <c r="H1" s="576"/>
-      <c r="I1" s="576"/>
-      <c r="J1" s="576"/>
-      <c r="K1" s="576"/>
-      <c r="L1" s="576"/>
-      <c r="M1" s="576"/>
+      <c r="B1" s="508"/>
+      <c r="C1" s="574" t="s">
+        <v>646</v>
+      </c>
+      <c r="D1" s="575"/>
+      <c r="E1" s="575"/>
+      <c r="F1" s="575"/>
+      <c r="G1" s="575"/>
+      <c r="H1" s="575"/>
+      <c r="I1" s="575"/>
+      <c r="J1" s="575"/>
+      <c r="K1" s="575"/>
+      <c r="L1" s="575"/>
+      <c r="M1" s="575"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="510"/>
+      <c r="B2" s="509"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -41201,24 +41255,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="513" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="514"/>
+      <c r="B3" s="512" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="513"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="515" t="s">
+      <c r="H3" s="514" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="515"/>
+      <c r="I3" s="514"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="552" t="s">
+      <c r="P3" s="551" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="573" t="s">
+      <c r="R3" s="572" t="s">
         <v>216</v>
       </c>
     </row>
@@ -41233,14 +41287,14 @@
       <c r="D4" s="18">
         <v>44591</v>
       </c>
-      <c r="E4" s="516" t="s">
+      <c r="E4" s="515" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="517"/>
-      <c r="H4" s="518" t="s">
+      <c r="F4" s="516"/>
+      <c r="H4" s="517" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="519"/>
+      <c r="I4" s="518"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -41250,15 +41304,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="553"/>
+      <c r="P4" s="552"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="574"/>
-      <c r="W4" s="562" t="s">
+      <c r="R4" s="573"/>
+      <c r="W4" s="561" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="562"/>
+      <c r="X4" s="561"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -41309,8 +41363,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="562"/>
-      <c r="X5" s="562"/>
+      <c r="W5" s="561"/>
+      <c r="X5" s="561"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -42071,7 +42125,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="566">
+      <c r="W19" s="565">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -42123,7 +42177,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="567"/>
+      <c r="W20" s="566"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -42172,8 +42226,8 @@
         <v>18072</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="568"/>
-      <c r="X21" s="568"/>
+      <c r="W21" s="567"/>
+      <c r="X21" s="567"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -42272,8 +42326,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="569"/>
-      <c r="X23" s="569"/>
+      <c r="W23" s="568"/>
+      <c r="X23" s="568"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -42328,8 +42382,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="569"/>
-      <c r="X24" s="569"/>
+      <c r="W24" s="568"/>
+      <c r="X24" s="568"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -42377,8 +42431,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="570"/>
-      <c r="X25" s="570"/>
+      <c r="W25" s="569"/>
+      <c r="X25" s="569"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -42426,8 +42480,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="570"/>
-      <c r="X26" s="570"/>
+      <c r="W26" s="569"/>
+      <c r="X26" s="569"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -42475,9 +42529,9 @@
       <c r="R27" s="319">
         <v>0</v>
       </c>
-      <c r="W27" s="563"/>
-      <c r="X27" s="564"/>
-      <c r="Y27" s="565"/>
+      <c r="W27" s="562"/>
+      <c r="X27" s="563"/>
+      <c r="Y27" s="564"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -42525,9 +42579,9 @@
       <c r="R28" s="319">
         <v>0</v>
       </c>
-      <c r="W28" s="564"/>
-      <c r="X28" s="564"/>
-      <c r="Y28" s="565"/>
+      <c r="W28" s="563"/>
+      <c r="X28" s="563"/>
+      <c r="Y28" s="564"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -42868,11 +42922,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="554">
+      <c r="M36" s="553">
         <f>SUM(M5:M35)</f>
         <v>2143864.4900000002</v>
       </c>
-      <c r="N36" s="556">
+      <c r="N36" s="555">
         <f>SUM(N5:N35)</f>
         <v>791108</v>
       </c>
@@ -42880,7 +42934,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="600">
+      <c r="Q36" s="599">
         <f>SUM(Q5:Q35)</f>
         <v>111.43999999999505</v>
       </c>
@@ -42905,13 +42959,13 @@
       <c r="L37" s="61">
         <v>16518.78</v>
       </c>
-      <c r="M37" s="555"/>
-      <c r="N37" s="557"/>
+      <c r="M37" s="554"/>
+      <c r="N37" s="556"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="601"/>
+      <c r="Q37" s="600"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -42961,11 +43015,11 @@
       <c r="L39" s="61">
         <v>14981.03</v>
       </c>
-      <c r="M39" s="602">
+      <c r="M39" s="601">
         <f>M36+N36</f>
         <v>2934972.49</v>
       </c>
-      <c r="N39" s="603"/>
+      <c r="N39" s="602"/>
       <c r="P39" s="34">
         <f>SUM(P5:P38)</f>
         <v>3450079.65</v>
@@ -43213,26 +43267,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="531" t="s">
+      <c r="H52" s="530" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="532"/>
+      <c r="I52" s="531"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="533">
+      <c r="K52" s="532">
         <f>I50+L50</f>
         <v>197471.8</v>
       </c>
-      <c r="L52" s="560"/>
+      <c r="L52" s="559"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="537" t="s">
+      <c r="D53" s="536" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="537"/>
+      <c r="E53" s="536"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>2057786.11</v>
@@ -43241,22 +43295,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="561" t="s">
+      <c r="D54" s="560" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="561"/>
+      <c r="E54" s="560"/>
       <c r="F54" s="111">
         <v>-1702928.14</v>
       </c>
-      <c r="I54" s="538" t="s">
+      <c r="I54" s="537" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="539"/>
-      <c r="K54" s="540">
+      <c r="J54" s="538"/>
+      <c r="K54" s="539">
         <f>F56+F57+F58</f>
         <v>1147965.3400000003</v>
       </c>
-      <c r="L54" s="540"/>
+      <c r="L54" s="539"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -43297,11 +43351,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="542">
+      <c r="K56" s="541">
         <f>-C4</f>
         <v>-1149740.4099999999</v>
       </c>
-      <c r="L56" s="543"/>
+      <c r="L56" s="542"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -43318,22 +43372,22 @@
       <c r="C58" s="112">
         <v>44619</v>
       </c>
-      <c r="D58" s="520" t="s">
+      <c r="D58" s="519" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="521"/>
+      <c r="E58" s="520"/>
       <c r="F58" s="113">
         <v>1266568.45</v>
       </c>
-      <c r="I58" s="522" t="s">
+      <c r="I58" s="521" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="523"/>
-      <c r="K58" s="524">
+      <c r="J58" s="522"/>
+      <c r="K58" s="523">
         <f>K54+K56</f>
         <v>-1775.0699999995995</v>
       </c>
-      <c r="L58" s="524"/>
+      <c r="L58" s="523"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>

</xml_diff>

<commit_message>
CIERRE 4 MAY 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #04  ABRIL   2022/BALANCE    ZAVALETA   ABRIL  2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #04  ABRIL   2022/BALANCE    ZAVALETA   ABRIL  2022.xlsx
@@ -541,7 +541,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="659">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -2503,6 +2503,21 @@
   </si>
   <si>
     <t>POLLO-QUESOS-JAMON-</t>
+  </si>
+  <si>
+    <t>Jamon-Pollo-Chorizo-Longaniza-Queso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENCHILADA-POLLO-LONGANIZA  </t>
+  </si>
+  <si>
+    <t>Longaniza --QUESOS</t>
+  </si>
+  <si>
+    <t>POLLO-QUESOS-CREMA</t>
+  </si>
+  <si>
+    <t>NOMINA # 18</t>
   </si>
 </sst>
 </file>
@@ -4309,7 +4324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="624">
+  <cellXfs count="620">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -5332,6 +5347,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="47" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5650,14 +5667,8 @@
     <xf numFmtId="166" fontId="13" fillId="6" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="15" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="2" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="15" fontId="2" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -9081,23 +9092,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="534"/>
-      <c r="C1" s="536" t="s">
+      <c r="B1" s="536"/>
+      <c r="C1" s="538" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="537"/>
-      <c r="E1" s="537"/>
-      <c r="F1" s="537"/>
-      <c r="G1" s="537"/>
-      <c r="H1" s="537"/>
-      <c r="I1" s="537"/>
-      <c r="J1" s="537"/>
-      <c r="K1" s="537"/>
-      <c r="L1" s="537"/>
-      <c r="M1" s="537"/>
+      <c r="D1" s="539"/>
+      <c r="E1" s="539"/>
+      <c r="F1" s="539"/>
+      <c r="G1" s="539"/>
+      <c r="H1" s="539"/>
+      <c r="I1" s="539"/>
+      <c r="J1" s="539"/>
+      <c r="K1" s="539"/>
+      <c r="L1" s="539"/>
+      <c r="M1" s="539"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="535"/>
+      <c r="B2" s="537"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -9107,17 +9118,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="538" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="539"/>
+      <c r="B3" s="540" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="541"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="540" t="s">
+      <c r="H3" s="542" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="540"/>
+      <c r="I3" s="542"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -9131,14 +9142,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="541" t="s">
+      <c r="E4" s="543" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="542"/>
-      <c r="H4" s="543" t="s">
+      <c r="F4" s="544"/>
+      <c r="H4" s="545" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="544"/>
+      <c r="I4" s="546"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -9148,10 +9159,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="515" t="s">
+      <c r="P4" s="517" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="516"/>
+      <c r="Q4" s="518"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -10592,11 +10603,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="517">
+      <c r="M39" s="519">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="519">
+      <c r="N39" s="521">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -10622,8 +10633,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="518"/>
-      <c r="N40" s="520"/>
+      <c r="M40" s="520"/>
+      <c r="N40" s="522"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -10838,29 +10849,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="521" t="s">
+      <c r="H52" s="523" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="522"/>
+      <c r="I52" s="524"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="523">
+      <c r="K52" s="525">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="524"/>
-      <c r="M52" s="525">
+      <c r="L52" s="526"/>
+      <c r="M52" s="527">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="526"/>
+      <c r="N52" s="528"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="527" t="s">
+      <c r="D53" s="529" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="527"/>
+      <c r="E53" s="529"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -10871,22 +10882,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="527" t="s">
+      <c r="D54" s="529" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="527"/>
+      <c r="E54" s="529"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="528" t="s">
+      <c r="I54" s="530" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="529"/>
-      <c r="K54" s="530">
+      <c r="J54" s="531"/>
+      <c r="K54" s="532">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="531"/>
+      <c r="L54" s="533"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -10919,11 +10930,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="532">
+      <c r="K56" s="534">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="533"/>
+      <c r="L56" s="535"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -10940,22 +10951,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="510" t="s">
+      <c r="D58" s="512" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="511"/>
+      <c r="E58" s="513"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="512" t="s">
+      <c r="I58" s="514" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="513"/>
-      <c r="K58" s="514">
+      <c r="J58" s="515"/>
+      <c r="K58" s="516">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="514"/>
+      <c r="L58" s="516"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -13579,10 +13590,10 @@
         <f t="shared" si="3"/>
         <v>188840.46999999997</v>
       </c>
-      <c r="I76" s="606" t="s">
+      <c r="I76" s="608" t="s">
         <v>597</v>
       </c>
-      <c r="J76" s="607"/>
+      <c r="J76" s="609"/>
       <c r="K76" s="69"/>
       <c r="L76" s="148"/>
       <c r="M76" s="69"/>
@@ -13601,8 +13612,8 @@
         <f t="shared" si="3"/>
         <v>188840.46999999997</v>
       </c>
-      <c r="I77" s="608"/>
-      <c r="J77" s="609"/>
+      <c r="I77" s="610"/>
+      <c r="J77" s="611"/>
       <c r="K77" s="69"/>
       <c r="L77" s="148"/>
       <c r="M77" s="69"/>
@@ -13669,7 +13680,7 @@
       <c r="C80" s="214"/>
       <c r="D80" s="256"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="572" t="s">
+      <c r="F80" s="574" t="s">
         <v>207</v>
       </c>
       <c r="K80" s="1"/>
@@ -13684,7 +13695,7 @@
       <c r="C81" s="463"/>
       <c r="D81" s="464"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="573"/>
+      <c r="F81" s="575"/>
       <c r="K81" s="1"/>
       <c r="L81" s="97"/>
       <c r="M81" s="3"/>
@@ -13692,10 +13703,10 @@
     </row>
     <row r="82" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A82" s="435"/>
-      <c r="B82" s="605" t="s">
+      <c r="B82" s="607" t="s">
         <v>595</v>
       </c>
-      <c r="C82" s="605"/>
+      <c r="C82" s="607"/>
       <c r="I82"/>
       <c r="J82" s="194"/>
     </row>
@@ -13977,23 +13988,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="534"/>
-      <c r="C1" s="576" t="s">
+      <c r="B1" s="536"/>
+      <c r="C1" s="578" t="s">
         <v>451</v>
       </c>
-      <c r="D1" s="577"/>
-      <c r="E1" s="577"/>
-      <c r="F1" s="577"/>
-      <c r="G1" s="577"/>
-      <c r="H1" s="577"/>
-      <c r="I1" s="577"/>
-      <c r="J1" s="577"/>
-      <c r="K1" s="577"/>
-      <c r="L1" s="577"/>
-      <c r="M1" s="577"/>
+      <c r="D1" s="579"/>
+      <c r="E1" s="579"/>
+      <c r="F1" s="579"/>
+      <c r="G1" s="579"/>
+      <c r="H1" s="579"/>
+      <c r="I1" s="579"/>
+      <c r="J1" s="579"/>
+      <c r="K1" s="579"/>
+      <c r="L1" s="579"/>
+      <c r="M1" s="579"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="535"/>
+      <c r="B2" s="537"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -14003,24 +14014,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="538" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="539"/>
+      <c r="B3" s="540" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="541"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="540" t="s">
+      <c r="H3" s="542" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="540"/>
+      <c r="I3" s="542"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="564" t="s">
+      <c r="P3" s="566" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="574" t="s">
+      <c r="R3" s="576" t="s">
         <v>216</v>
       </c>
     </row>
@@ -14035,14 +14046,14 @@
       <c r="D4" s="18">
         <v>44619</v>
       </c>
-      <c r="E4" s="541" t="s">
+      <c r="E4" s="543" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="542"/>
-      <c r="H4" s="543" t="s">
+      <c r="F4" s="544"/>
+      <c r="H4" s="545" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="544"/>
+      <c r="I4" s="546"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -14052,15 +14063,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="565"/>
+      <c r="P4" s="567"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="575"/>
-      <c r="W4" s="547" t="s">
+      <c r="R4" s="577"/>
+      <c r="W4" s="549" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="547"/>
+      <c r="X4" s="549"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -14111,8 +14122,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="547"/>
-      <c r="X5" s="547"/>
+      <c r="W5" s="549"/>
+      <c r="X5" s="549"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -14875,7 +14886,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="551">
+      <c r="W19" s="553">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -14927,7 +14938,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="552"/>
+      <c r="W20" s="554"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -14976,8 +14987,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="553"/>
-      <c r="X21" s="553"/>
+      <c r="W21" s="555"/>
+      <c r="X21" s="555"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -15077,8 +15088,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="554"/>
-      <c r="X23" s="554"/>
+      <c r="W23" s="556"/>
+      <c r="X23" s="556"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -15133,8 +15144,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="554"/>
-      <c r="X24" s="554"/>
+      <c r="W24" s="556"/>
+      <c r="X24" s="556"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -15182,8 +15193,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="555"/>
-      <c r="X25" s="555"/>
+      <c r="W25" s="557"/>
+      <c r="X25" s="557"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -15232,8 +15243,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="555"/>
-      <c r="X26" s="555"/>
+      <c r="W26" s="557"/>
+      <c r="X26" s="557"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -15281,9 +15292,9 @@
       <c r="R27" s="388">
         <v>170</v>
       </c>
-      <c r="W27" s="548"/>
-      <c r="X27" s="549"/>
-      <c r="Y27" s="550"/>
+      <c r="W27" s="550"/>
+      <c r="X27" s="551"/>
+      <c r="Y27" s="552"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -15331,9 +15342,9 @@
       <c r="R28" s="388">
         <v>37374.36</v>
       </c>
-      <c r="W28" s="549"/>
-      <c r="X28" s="549"/>
-      <c r="Y28" s="550"/>
+      <c r="W28" s="551"/>
+      <c r="X28" s="551"/>
+      <c r="Y28" s="552"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -15665,11 +15676,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="566">
+      <c r="M36" s="568">
         <f>SUM(M5:M35)</f>
         <v>2220612.02</v>
       </c>
-      <c r="N36" s="568">
+      <c r="N36" s="570">
         <f>SUM(N5:N35)</f>
         <v>833865</v>
       </c>
@@ -15677,7 +15688,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="601">
+      <c r="Q36" s="603">
         <f>SUM(Q5:Q35)</f>
         <v>8.3000000000320142</v>
       </c>
@@ -15702,13 +15713,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="567"/>
-      <c r="N37" s="569"/>
+      <c r="M37" s="569"/>
+      <c r="N37" s="571"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="602"/>
+      <c r="Q37" s="604"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -15753,11 +15764,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="603">
+      <c r="M39" s="605">
         <f>M36+N36</f>
         <v>3054477.02</v>
       </c>
-      <c r="N39" s="604"/>
+      <c r="N39" s="606"/>
       <c r="P39" s="34">
         <f>SUM(P5:P38)</f>
         <v>3627989.66</v>
@@ -16017,26 +16028,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="521" t="s">
+      <c r="H52" s="523" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="522"/>
+      <c r="I52" s="524"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="523">
+      <c r="K52" s="525">
         <f>I50+L50</f>
         <v>217159.4</v>
       </c>
-      <c r="L52" s="556"/>
+      <c r="L52" s="558"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="527" t="s">
+      <c r="D53" s="529" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="527"/>
+      <c r="E53" s="529"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>1453241.94</v>
@@ -16045,22 +16056,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="557" t="s">
+      <c r="D54" s="559" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="557"/>
+      <c r="E54" s="559"/>
       <c r="F54" s="111">
         <v>-1360260.32</v>
       </c>
-      <c r="I54" s="528" t="s">
+      <c r="I54" s="530" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="529"/>
-      <c r="K54" s="530">
+      <c r="J54" s="531"/>
+      <c r="K54" s="532">
         <f>F56+F57+F58</f>
         <v>1797288.1999999997</v>
       </c>
-      <c r="L54" s="530"/>
+      <c r="L54" s="532"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -16101,11 +16112,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="532">
+      <c r="K56" s="534">
         <f>-C4</f>
         <v>-1266568.45</v>
       </c>
-      <c r="L56" s="533"/>
+      <c r="L56" s="535"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -16122,22 +16133,22 @@
       <c r="C58" s="112">
         <v>44647</v>
       </c>
-      <c r="D58" s="510" t="s">
+      <c r="D58" s="512" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="511"/>
+      <c r="E58" s="513"/>
       <c r="F58" s="113">
         <v>1792817.68</v>
       </c>
-      <c r="I58" s="512" t="s">
+      <c r="I58" s="514" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="513"/>
-      <c r="K58" s="514">
+      <c r="J58" s="515"/>
+      <c r="K58" s="516">
         <f>K54+K56</f>
         <v>530719.74999999977</v>
       </c>
-      <c r="L58" s="514"/>
+      <c r="L58" s="516"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -18489,7 +18500,7 @@
       <c r="C80" s="214"/>
       <c r="D80" s="256"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="572" t="s">
+      <c r="F80" s="574" t="s">
         <v>207</v>
       </c>
       <c r="K80" s="1"/>
@@ -18502,7 +18513,7 @@
       <c r="C81" s="1"/>
       <c r="D81" s="256"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="573"/>
+      <c r="F81" s="575"/>
       <c r="K81" s="1"/>
       <c r="L81" s="97"/>
       <c r="M81" s="3"/>
@@ -18522,16 +18533,16 @@
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="456"/>
       <c r="B83" s="442"/>
-      <c r="I83" s="610" t="s">
+      <c r="I83" s="612" t="s">
         <v>594</v>
       </c>
-      <c r="J83" s="611"/>
+      <c r="J83" s="613"/>
     </row>
     <row r="84" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="456"/>
       <c r="B84" s="442"/>
-      <c r="I84" s="612"/>
-      <c r="J84" s="613"/>
+      <c r="I84" s="614"/>
+      <c r="J84" s="615"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="456"/>
@@ -18798,8 +18809,8 @@
   </sheetPr>
   <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I25" workbookViewId="0">
-      <selection activeCell="Q35" sqref="Q35"/>
+    <sheetView tabSelected="1" topLeftCell="H25" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -18816,7 +18827,7 @@
     <col min="11" max="11" width="14.42578125" style="162" customWidth="1"/>
     <col min="12" max="12" width="14.5703125" style="3" customWidth="1"/>
     <col min="13" max="13" width="17.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.85546875" customWidth="1"/>
     <col min="17" max="17" width="21.28515625" style="225" customWidth="1"/>
@@ -18828,23 +18839,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="534"/>
-      <c r="C1" s="576" t="s">
+      <c r="B1" s="536"/>
+      <c r="C1" s="578" t="s">
         <v>620</v>
       </c>
-      <c r="D1" s="577"/>
-      <c r="E1" s="577"/>
-      <c r="F1" s="577"/>
-      <c r="G1" s="577"/>
-      <c r="H1" s="577"/>
-      <c r="I1" s="577"/>
-      <c r="J1" s="577"/>
-      <c r="K1" s="577"/>
-      <c r="L1" s="577"/>
-      <c r="M1" s="577"/>
+      <c r="D1" s="579"/>
+      <c r="E1" s="579"/>
+      <c r="F1" s="579"/>
+      <c r="G1" s="579"/>
+      <c r="H1" s="579"/>
+      <c r="I1" s="579"/>
+      <c r="J1" s="579"/>
+      <c r="K1" s="579"/>
+      <c r="L1" s="579"/>
+      <c r="M1" s="579"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="535"/>
+      <c r="B2" s="537"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -18854,24 +18865,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="538" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="539"/>
+      <c r="B3" s="540" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="541"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="540" t="s">
+      <c r="H3" s="542" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="540"/>
+      <c r="I3" s="542"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="564" t="s">
+      <c r="P3" s="566" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="574" t="s">
+      <c r="R3" s="576" t="s">
         <v>216</v>
       </c>
     </row>
@@ -18886,14 +18897,14 @@
       <c r="D4" s="18">
         <v>44647</v>
       </c>
-      <c r="E4" s="541" t="s">
+      <c r="E4" s="543" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="542"/>
-      <c r="H4" s="543" t="s">
+      <c r="F4" s="544"/>
+      <c r="H4" s="545" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="544"/>
+      <c r="I4" s="546"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -18903,15 +18914,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="565"/>
+      <c r="P4" s="567"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="575"/>
-      <c r="W4" s="547" t="s">
+      <c r="R4" s="577"/>
+      <c r="W4" s="549" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="547"/>
+      <c r="X4" s="549"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -18962,8 +18973,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="547"/>
-      <c r="X5" s="547"/>
+      <c r="W5" s="549"/>
+      <c r="X5" s="549"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -19722,7 +19733,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="551">
+      <c r="W19" s="553">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -19774,7 +19785,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="552"/>
+      <c r="W20" s="554"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -19823,8 +19834,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="553"/>
-      <c r="X21" s="553"/>
+      <c r="W21" s="555"/>
+      <c r="X21" s="555"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -19921,8 +19932,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="554"/>
-      <c r="X23" s="554"/>
+      <c r="W23" s="556"/>
+      <c r="X23" s="556"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -19977,8 +19988,8 @@
         <v>642</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="554"/>
-      <c r="X24" s="554"/>
+      <c r="W24" s="556"/>
+      <c r="X24" s="556"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -20024,8 +20035,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="555"/>
-      <c r="X25" s="555"/>
+      <c r="W25" s="557"/>
+      <c r="X25" s="557"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -20074,8 +20085,8 @@
       <c r="R26" s="388">
         <v>73524.61</v>
       </c>
-      <c r="W26" s="555"/>
-      <c r="X26" s="555"/>
+      <c r="W26" s="557"/>
+      <c r="X26" s="557"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -20124,9 +20135,9 @@
       <c r="R27" s="319">
         <v>0</v>
       </c>
-      <c r="W27" s="548"/>
-      <c r="X27" s="549"/>
-      <c r="Y27" s="550"/>
+      <c r="W27" s="550"/>
+      <c r="X27" s="551"/>
+      <c r="Y27" s="552"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -20174,9 +20185,9 @@
       <c r="R28" s="319">
         <v>0</v>
       </c>
-      <c r="W28" s="549"/>
-      <c r="X28" s="549"/>
-      <c r="Y28" s="550"/>
+      <c r="W28" s="551"/>
+      <c r="X28" s="551"/>
+      <c r="Y28" s="552"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -20432,7 +20443,9 @@
         <f t="shared" ref="Q33:Q40" si="2">P33-F33</f>
         <v>0</v>
       </c>
-      <c r="R33" s="228"/>
+      <c r="R33" s="319">
+        <v>0</v>
+      </c>
       <c r="T33" s="424">
         <f>SUM(T29:T32)</f>
         <v>44254</v>
@@ -20443,36 +20456,46 @@
       <c r="B34" s="24">
         <v>44677</v>
       </c>
-      <c r="C34" s="617"/>
-      <c r="D34" s="618"/>
-      <c r="E34" s="619">
+      <c r="C34" s="25">
+        <v>13489</v>
+      </c>
+      <c r="D34" s="64" t="s">
+        <v>654</v>
+      </c>
+      <c r="E34" s="27">
         <v>44677</v>
       </c>
-      <c r="F34" s="620"/>
-      <c r="G34" s="621"/>
-      <c r="H34" s="622">
+      <c r="F34" s="28">
+        <v>77669</v>
+      </c>
+      <c r="G34" s="2"/>
+      <c r="H34" s="36">
         <v>44677</v>
       </c>
-      <c r="I34" s="623"/>
+      <c r="I34" s="30">
+        <v>879.5</v>
+      </c>
       <c r="J34" s="266"/>
       <c r="K34" s="248"/>
       <c r="L34" s="44"/>
       <c r="M34" s="32">
-        <v>0</v>
+        <f>40390+4760</f>
+        <v>45150</v>
       </c>
       <c r="N34" s="33">
-        <v>0</v>
+        <v>22911</v>
       </c>
       <c r="O34" s="2"/>
       <c r="P34" s="34">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>82429.5</v>
       </c>
       <c r="Q34" s="111">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R34" s="228"/>
+        <v>0</v>
+      </c>
+      <c r="R34" s="388">
+        <v>4760</v>
+      </c>
     </row>
     <row r="35" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="23"/>
@@ -20515,80 +20538,100 @@
         <f t="shared" si="2"/>
         <v>-2</v>
       </c>
-      <c r="R35" s="228"/>
+      <c r="R35" s="319">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="23"/>
       <c r="B36" s="24">
         <v>44679</v>
       </c>
-      <c r="C36" s="25"/>
-      <c r="D36" s="62"/>
+      <c r="C36" s="25">
+        <v>16710</v>
+      </c>
+      <c r="D36" s="67" t="s">
+        <v>655</v>
+      </c>
       <c r="E36" s="27">
         <v>44679</v>
       </c>
-      <c r="F36" s="28"/>
+      <c r="F36" s="28">
+        <v>149331</v>
+      </c>
       <c r="G36" s="2"/>
       <c r="H36" s="36">
         <v>44679</v>
       </c>
-      <c r="I36" s="30"/>
+      <c r="I36" s="30">
+        <v>3361</v>
+      </c>
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
       <c r="M36" s="267">
-        <v>0</v>
+        <v>99132</v>
       </c>
       <c r="N36" s="268">
-        <v>0</v>
+        <v>29993</v>
       </c>
       <c r="O36" s="276"/>
       <c r="P36" s="34">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q36" s="111">
+        <v>149196</v>
+      </c>
+      <c r="Q36" s="511">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R36" s="228"/>
+        <v>-135</v>
+      </c>
+      <c r="R36" s="319">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="23"/>
       <c r="B37" s="24">
         <v>44680</v>
       </c>
-      <c r="C37" s="25"/>
-      <c r="D37" s="65"/>
+      <c r="C37" s="25">
+        <v>10619</v>
+      </c>
+      <c r="D37" s="64" t="s">
+        <v>656</v>
+      </c>
       <c r="E37" s="27">
         <v>44680</v>
       </c>
-      <c r="F37" s="28"/>
+      <c r="F37" s="28">
+        <v>134928</v>
+      </c>
       <c r="G37" s="2"/>
       <c r="H37" s="36">
         <v>44680</v>
       </c>
-      <c r="I37" s="30"/>
+      <c r="I37" s="30">
+        <v>3150</v>
+      </c>
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
       <c r="M37" s="267">
-        <v>0</v>
+        <v>73283</v>
       </c>
       <c r="N37" s="268">
-        <v>0</v>
+        <v>47876</v>
       </c>
       <c r="O37" s="276"/>
       <c r="P37" s="34">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>134928</v>
       </c>
       <c r="Q37" s="111">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R37" s="227" t="s">
-        <v>7</v>
+      <c r="R37" s="319">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -20596,32 +20639,49 @@
       <c r="B38" s="24">
         <v>44681</v>
       </c>
-      <c r="C38" s="25"/>
-      <c r="D38" s="65"/>
+      <c r="C38" s="25">
+        <v>9895</v>
+      </c>
+      <c r="D38" s="618" t="s">
+        <v>657</v>
+      </c>
       <c r="E38" s="27">
         <v>44681</v>
       </c>
-      <c r="F38" s="28"/>
+      <c r="F38" s="28">
+        <v>148944</v>
+      </c>
       <c r="G38" s="2"/>
       <c r="H38" s="36">
         <v>44681</v>
       </c>
-      <c r="I38" s="30"/>
-      <c r="J38" s="60"/>
-      <c r="K38" s="177"/>
-      <c r="L38" s="61"/>
+      <c r="I38" s="30">
+        <v>4895</v>
+      </c>
+      <c r="J38" s="60">
+        <v>44681</v>
+      </c>
+      <c r="K38" s="177" t="s">
+        <v>658</v>
+      </c>
+      <c r="L38" s="61">
+        <v>20352</v>
+      </c>
       <c r="M38" s="267">
-        <v>0</v>
+        <v>51036</v>
       </c>
       <c r="N38" s="268">
-        <v>0</v>
+        <v>62766</v>
       </c>
       <c r="P38" s="34">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>N38+M38+L38+I38+C38</f>
+        <v>148944</v>
       </c>
       <c r="Q38" s="111">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R38" s="319">
         <v>0</v>
       </c>
     </row>
@@ -20631,7 +20691,7 @@
         <v>44682</v>
       </c>
       <c r="C39" s="69"/>
-      <c r="D39" s="62"/>
+      <c r="D39" s="618"/>
       <c r="E39" s="27">
         <v>44682</v>
       </c>
@@ -20658,12 +20718,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="R39" s="319">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="23"/>
       <c r="B40" s="24"/>
       <c r="C40" s="69"/>
-      <c r="D40" s="62"/>
+      <c r="D40" s="618"/>
       <c r="E40" s="27"/>
       <c r="F40" s="70"/>
       <c r="G40" s="2"/>
@@ -20686,12 +20749,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="R40" s="319">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="23"/>
       <c r="B41" s="24"/>
       <c r="C41" s="72"/>
-      <c r="D41" s="73"/>
+      <c r="D41" s="619"/>
       <c r="E41" s="74"/>
       <c r="F41" s="75"/>
       <c r="G41" s="2"/>
@@ -20706,28 +20772,28 @@
       <c r="L41" s="61">
         <v>15798.5</v>
       </c>
-      <c r="M41" s="566">
+      <c r="M41" s="568">
         <f>SUM(M5:M40)</f>
-        <v>2078201.61</v>
-      </c>
-      <c r="N41" s="566">
+        <v>2346802.6100000003</v>
+      </c>
+      <c r="N41" s="568">
         <f>SUM(N5:N40)</f>
-        <v>996536</v>
-      </c>
-      <c r="P41" s="616">
+        <v>1160082</v>
+      </c>
+      <c r="P41" s="510">
         <f>SUM(P5:P40)</f>
-        <v>3661561.2399999998</v>
-      </c>
-      <c r="Q41" s="601">
+        <v>4177058.7399999998</v>
+      </c>
+      <c r="Q41" s="603">
         <f>SUM(Q5:Q40)</f>
-        <v>-0.3700000000098953</v>
+        <v>-135.3700000000099</v>
       </c>
     </row>
     <row r="42" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="23"/>
       <c r="B42" s="24"/>
       <c r="C42" s="72"/>
-      <c r="D42" s="73"/>
+      <c r="D42" s="619"/>
       <c r="E42" s="74"/>
       <c r="F42" s="75"/>
       <c r="G42" s="2"/>
@@ -20742,16 +20808,16 @@
       <c r="L42" s="52">
         <v>15298.5</v>
       </c>
-      <c r="M42" s="567"/>
-      <c r="N42" s="567"/>
+      <c r="M42" s="569"/>
+      <c r="N42" s="569"/>
       <c r="P42" s="34"/>
-      <c r="Q42" s="602"/>
+      <c r="Q42" s="604"/>
     </row>
     <row r="43" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="23"/>
       <c r="B43" s="24"/>
       <c r="C43" s="72"/>
-      <c r="D43" s="73"/>
+      <c r="D43" s="619"/>
       <c r="E43" s="74"/>
       <c r="F43" s="75"/>
       <c r="G43" s="2"/>
@@ -20775,7 +20841,7 @@
       <c r="A44" s="23"/>
       <c r="B44" s="24"/>
       <c r="C44" s="72"/>
-      <c r="D44" s="73"/>
+      <c r="D44" s="619"/>
       <c r="E44" s="74"/>
       <c r="F44" s="75"/>
       <c r="G44" s="2"/>
@@ -20800,20 +20866,26 @@
       <c r="A45" s="23"/>
       <c r="B45" s="24"/>
       <c r="C45" s="72"/>
-      <c r="D45" s="73"/>
+      <c r="D45" s="619"/>
       <c r="E45" s="74"/>
       <c r="F45" s="75"/>
       <c r="G45" s="2"/>
       <c r="H45" s="76"/>
       <c r="I45" s="77"/>
-      <c r="J45" s="60"/>
-      <c r="K45" s="41"/>
-      <c r="L45" s="61"/>
-      <c r="M45" s="614">
+      <c r="J45" s="60">
+        <v>44681</v>
+      </c>
+      <c r="K45" s="41" t="s">
+        <v>658</v>
+      </c>
+      <c r="L45" s="61">
+        <v>18269.490000000002</v>
+      </c>
+      <c r="M45" s="616">
         <f>M41+N41</f>
-        <v>3074737.6100000003</v>
-      </c>
-      <c r="N45" s="615"/>
+        <v>3506884.6100000003</v>
+      </c>
+      <c r="N45" s="617"/>
       <c r="P45" s="34"/>
       <c r="Q45" s="13"/>
     </row>
@@ -20821,7 +20893,7 @@
       <c r="A46" s="23"/>
       <c r="B46" s="24"/>
       <c r="C46" s="72"/>
-      <c r="D46" s="73"/>
+      <c r="D46" s="619"/>
       <c r="E46" s="74"/>
       <c r="F46" s="75"/>
       <c r="G46" s="2"/>
@@ -20839,7 +20911,7 @@
       <c r="A47" s="23"/>
       <c r="B47" s="24"/>
       <c r="C47" s="72"/>
-      <c r="D47" s="73"/>
+      <c r="D47" s="619"/>
       <c r="E47" s="74"/>
       <c r="F47" s="75"/>
       <c r="G47" s="2"/>
@@ -20896,7 +20968,7 @@
       </c>
       <c r="C50" s="87">
         <f>SUM(C5:C49)</f>
-        <v>418372.5</v>
+        <v>469085.5</v>
       </c>
       <c r="D50" s="88"/>
       <c r="E50" s="89" t="s">
@@ -20904,7 +20976,7 @@
       </c>
       <c r="F50" s="90">
         <f>SUM(F5:F49)</f>
-        <v>3548546</v>
+        <v>4059418</v>
       </c>
       <c r="G50" s="88"/>
       <c r="H50" s="91" t="s">
@@ -20912,7 +20984,7 @@
       </c>
       <c r="I50" s="92">
         <f>SUM(I5:I49)</f>
-        <v>87149.5</v>
+        <v>99435</v>
       </c>
       <c r="J50" s="93"/>
       <c r="K50" s="94" t="s">
@@ -20920,7 +20992,7 @@
       </c>
       <c r="L50" s="95">
         <f>SUM(L5:L49)</f>
-        <v>147517.34000000003</v>
+        <v>186138.83000000002</v>
       </c>
       <c r="M50" s="96"/>
       <c r="N50" s="96"/>
@@ -20938,50 +21010,50 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="521" t="s">
+      <c r="H52" s="523" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="522"/>
+      <c r="I52" s="524"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="523">
+      <c r="K52" s="525">
         <f>I50+L50</f>
-        <v>234666.84000000003</v>
-      </c>
-      <c r="L52" s="556"/>
+        <v>285573.83</v>
+      </c>
+      <c r="L52" s="558"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="527" t="s">
+      <c r="D53" s="529" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="527"/>
+      <c r="E53" s="529"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
-        <v>2895506.66</v>
+        <v>3304758.67</v>
       </c>
       <c r="I53" s="102"/>
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="557" t="s">
+      <c r="D54" s="559" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="557"/>
+      <c r="E54" s="559"/>
       <c r="F54" s="111">
         <v>0</v>
       </c>
-      <c r="I54" s="528" t="s">
+      <c r="I54" s="530" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="529"/>
-      <c r="K54" s="530">
+      <c r="J54" s="531"/>
+      <c r="K54" s="532">
         <f>F56+F57+F58</f>
-        <v>2895506.66</v>
-      </c>
-      <c r="L54" s="530"/>
+        <v>3304758.67</v>
+      </c>
+      <c r="L54" s="532"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -21015,18 +21087,18 @@
       </c>
       <c r="F56" s="96">
         <f>SUM(F53:F55)</f>
-        <v>2895506.66</v>
+        <v>3304758.67</v>
       </c>
       <c r="H56" s="23"/>
       <c r="I56" s="108" t="s">
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="532">
+      <c r="K56" s="534">
         <f>-C4</f>
         <v>-1792817.68</v>
       </c>
-      <c r="L56" s="533"/>
+      <c r="L56" s="535"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -21041,22 +21113,22 @@
     </row>
     <row r="58" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C58" s="112"/>
-      <c r="D58" s="510" t="s">
+      <c r="D58" s="512" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="511"/>
+      <c r="E58" s="513"/>
       <c r="F58" s="113">
         <v>0</v>
       </c>
-      <c r="I58" s="512" t="s">
+      <c r="I58" s="514" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="513"/>
-      <c r="K58" s="514">
+      <c r="J58" s="515"/>
+      <c r="K58" s="516">
         <f>K54+K56</f>
-        <v>1102688.9800000002</v>
-      </c>
-      <c r="L58" s="514"/>
+        <v>1511940.99</v>
+      </c>
+      <c r="L58" s="516"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -22891,7 +22963,7 @@
       <c r="C80" s="214"/>
       <c r="D80" s="256"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="572" t="s">
+      <c r="F80" s="574" t="s">
         <v>207</v>
       </c>
       <c r="K80" s="1"/>
@@ -22904,7 +22976,7 @@
       <c r="C81" s="1"/>
       <c r="D81" s="256"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="573"/>
+      <c r="F81" s="575"/>
       <c r="K81" s="1"/>
       <c r="L81" s="97"/>
       <c r="M81" s="3"/>
@@ -22923,16 +22995,16 @@
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="456"/>
       <c r="B83" s="442"/>
-      <c r="I83" s="610" t="s">
+      <c r="I83" s="612" t="s">
         <v>594</v>
       </c>
-      <c r="J83" s="611"/>
+      <c r="J83" s="613"/>
     </row>
     <row r="84" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="456"/>
       <c r="B84" s="442"/>
-      <c r="I84" s="612"/>
-      <c r="J84" s="613"/>
+      <c r="I84" s="614"/>
+      <c r="J84" s="615"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="456"/>
@@ -24549,7 +24621,7 @@
       <c r="A41" s="140">
         <v>44507</v>
       </c>
-      <c r="B41" s="545" t="s">
+      <c r="B41" s="547" t="s">
         <v>92</v>
       </c>
       <c r="C41" s="190">
@@ -24581,7 +24653,7 @@
       <c r="A42" s="140" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="546"/>
+      <c r="B42" s="548"/>
       <c r="C42" s="143">
         <v>0</v>
       </c>
@@ -26177,23 +26249,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="534"/>
-      <c r="C1" s="536" t="s">
+      <c r="B1" s="536"/>
+      <c r="C1" s="538" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="537"/>
-      <c r="E1" s="537"/>
-      <c r="F1" s="537"/>
-      <c r="G1" s="537"/>
-      <c r="H1" s="537"/>
-      <c r="I1" s="537"/>
-      <c r="J1" s="537"/>
-      <c r="K1" s="537"/>
-      <c r="L1" s="537"/>
-      <c r="M1" s="537"/>
+      <c r="D1" s="539"/>
+      <c r="E1" s="539"/>
+      <c r="F1" s="539"/>
+      <c r="G1" s="539"/>
+      <c r="H1" s="539"/>
+      <c r="I1" s="539"/>
+      <c r="J1" s="539"/>
+      <c r="K1" s="539"/>
+      <c r="L1" s="539"/>
+      <c r="M1" s="539"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="535"/>
+      <c r="B2" s="537"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -26203,21 +26275,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="538" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="539"/>
+      <c r="B3" s="540" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="541"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="540" t="s">
+      <c r="H3" s="542" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="540"/>
+      <c r="I3" s="542"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="564" t="s">
+      <c r="P3" s="566" t="s">
         <v>6</v>
       </c>
     </row>
@@ -26232,14 +26304,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="541" t="s">
+      <c r="E4" s="543" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="542"/>
-      <c r="H4" s="543" t="s">
+      <c r="F4" s="544"/>
+      <c r="H4" s="545" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="544"/>
+      <c r="I4" s="546"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -26249,14 +26321,14 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="565"/>
+      <c r="P4" s="567"/>
       <c r="Q4" s="286" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="547" t="s">
+      <c r="W4" s="549" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="547"/>
+      <c r="X4" s="549"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -26307,8 +26379,8 @@
         <f>20000+7936</f>
         <v>27936</v>
       </c>
-      <c r="W5" s="547"/>
-      <c r="X5" s="547"/>
+      <c r="W5" s="549"/>
+      <c r="X5" s="549"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -27079,7 +27151,7 @@
         <v>26370</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="551">
+      <c r="W19" s="553">
         <f>SUM(W6:W18)</f>
         <v>935136</v>
       </c>
@@ -27131,7 +27203,7 @@
         <v>16395.830000000002</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="552"/>
+      <c r="W20" s="554"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -27180,8 +27252,8 @@
         <v>19188.82</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="553"/>
-      <c r="X21" s="553"/>
+      <c r="W21" s="555"/>
+      <c r="X21" s="555"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -27282,8 +27354,8 @@
         <v>45217.29</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="554"/>
-      <c r="X23" s="554"/>
+      <c r="W23" s="556"/>
+      <c r="X23" s="556"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -27337,8 +27409,8 @@
         <v>23159.17</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="554"/>
-      <c r="X24" s="554"/>
+      <c r="W24" s="556"/>
+      <c r="X24" s="556"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -27384,8 +27456,8 @@
       <c r="R25" s="285">
         <v>28952</v>
       </c>
-      <c r="W25" s="555"/>
-      <c r="X25" s="555"/>
+      <c r="W25" s="557"/>
+      <c r="X25" s="557"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -27436,8 +27508,8 @@
       <c r="R26" s="285">
         <v>21771.5</v>
       </c>
-      <c r="W26" s="555"/>
-      <c r="X26" s="555"/>
+      <c r="W26" s="557"/>
+      <c r="X26" s="557"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -27485,9 +27557,9 @@
       <c r="R27" s="285">
         <v>14637</v>
       </c>
-      <c r="W27" s="548"/>
-      <c r="X27" s="549"/>
-      <c r="Y27" s="550"/>
+      <c r="W27" s="550"/>
+      <c r="X27" s="551"/>
+      <c r="Y27" s="552"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -27537,9 +27609,9 @@
       <c r="R28" s="285">
         <v>0</v>
       </c>
-      <c r="W28" s="549"/>
-      <c r="X28" s="549"/>
-      <c r="Y28" s="550"/>
+      <c r="W28" s="551"/>
+      <c r="X28" s="551"/>
+      <c r="Y28" s="552"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -27874,11 +27946,11 @@
       <c r="L36" s="44">
         <v>5940</v>
       </c>
-      <c r="M36" s="566">
+      <c r="M36" s="568">
         <f>SUM(M5:M35)</f>
         <v>321168.83</v>
       </c>
-      <c r="N36" s="568">
+      <c r="N36" s="570">
         <f>SUM(N5:N35)</f>
         <v>467016</v>
       </c>
@@ -27886,7 +27958,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="570">
+      <c r="Q36" s="572">
         <f>SUM(Q5:Q35)</f>
         <v>-637069.14000000013</v>
       </c>
@@ -27921,13 +27993,13 @@
       <c r="L37" s="61">
         <v>7929.62</v>
       </c>
-      <c r="M37" s="567"/>
-      <c r="N37" s="569"/>
+      <c r="M37" s="569"/>
+      <c r="N37" s="571"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="571"/>
+      <c r="Q37" s="573"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -28217,26 +28289,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="521" t="s">
+      <c r="H52" s="523" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="522"/>
+      <c r="I52" s="524"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="523">
+      <c r="K52" s="525">
         <f>I50+L50</f>
         <v>71911.59</v>
       </c>
-      <c r="L52" s="556"/>
+      <c r="L52" s="558"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="527" t="s">
+      <c r="D53" s="529" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="527"/>
+      <c r="E53" s="529"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>-25952.549999999814</v>
@@ -28245,29 +28317,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="557" t="s">
+      <c r="D54" s="559" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="557"/>
+      <c r="E54" s="559"/>
       <c r="F54" s="111">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="528" t="s">
+      <c r="I54" s="530" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="529"/>
-      <c r="K54" s="530">
+      <c r="J54" s="531"/>
+      <c r="K54" s="532">
         <f>F56+F57+F58</f>
         <v>1308778.3500000003</v>
       </c>
-      <c r="L54" s="530"/>
-      <c r="M54" s="558" t="s">
+      <c r="L54" s="532"/>
+      <c r="M54" s="560" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="559"/>
-      <c r="O54" s="559"/>
-      <c r="P54" s="559"/>
-      <c r="Q54" s="560"/>
+      <c r="N54" s="561"/>
+      <c r="O54" s="561"/>
+      <c r="P54" s="561"/>
+      <c r="Q54" s="562"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="313" t="s">
@@ -28281,11 +28353,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="561"/>
-      <c r="N55" s="562"/>
-      <c r="O55" s="562"/>
-      <c r="P55" s="562"/>
-      <c r="Q55" s="563"/>
+      <c r="M55" s="563"/>
+      <c r="N55" s="564"/>
+      <c r="O55" s="564"/>
+      <c r="P55" s="564"/>
+      <c r="Q55" s="565"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -28303,11 +28375,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="532">
+      <c r="K56" s="534">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="533"/>
+      <c r="L56" s="535"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -28324,22 +28396,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="510" t="s">
+      <c r="D58" s="512" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="511"/>
+      <c r="E58" s="513"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="512" t="s">
+      <c r="I58" s="514" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="513"/>
-      <c r="K58" s="514">
+      <c r="J58" s="515"/>
+      <c r="K58" s="516">
         <f>K54+K56</f>
         <v>741389.00000000035</v>
       </c>
-      <c r="L58" s="514"/>
+      <c r="L58" s="516"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -30929,7 +31001,7 @@
       <c r="C87" s="214"/>
       <c r="D87" s="97"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="572" t="s">
+      <c r="F87" s="574" t="s">
         <v>207</v>
       </c>
       <c r="K87" s="1"/>
@@ -30942,7 +31014,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="97"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="573"/>
+      <c r="F88" s="575"/>
       <c r="K88" s="1"/>
       <c r="L88" s="256"/>
       <c r="M88" s="3"/>
@@ -31254,23 +31326,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="534"/>
-      <c r="C1" s="536" t="s">
+      <c r="B1" s="536"/>
+      <c r="C1" s="538" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="537"/>
-      <c r="E1" s="537"/>
-      <c r="F1" s="537"/>
-      <c r="G1" s="537"/>
-      <c r="H1" s="537"/>
-      <c r="I1" s="537"/>
-      <c r="J1" s="537"/>
-      <c r="K1" s="537"/>
-      <c r="L1" s="537"/>
-      <c r="M1" s="537"/>
+      <c r="D1" s="539"/>
+      <c r="E1" s="539"/>
+      <c r="F1" s="539"/>
+      <c r="G1" s="539"/>
+      <c r="H1" s="539"/>
+      <c r="I1" s="539"/>
+      <c r="J1" s="539"/>
+      <c r="K1" s="539"/>
+      <c r="L1" s="539"/>
+      <c r="M1" s="539"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="535"/>
+      <c r="B2" s="537"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -31280,24 +31352,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="538" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="539"/>
+      <c r="B3" s="540" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="541"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="540" t="s">
+      <c r="H3" s="542" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="540"/>
+      <c r="I3" s="542"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="564" t="s">
+      <c r="P3" s="566" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="574" t="s">
+      <c r="R3" s="576" t="s">
         <v>216</v>
       </c>
     </row>
@@ -31312,14 +31384,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="541" t="s">
+      <c r="E4" s="543" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="542"/>
-      <c r="H4" s="543" t="s">
+      <c r="F4" s="544"/>
+      <c r="H4" s="545" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="544"/>
+      <c r="I4" s="546"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -31329,15 +31401,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="565"/>
+      <c r="P4" s="567"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="575"/>
-      <c r="W4" s="547" t="s">
+      <c r="R4" s="577"/>
+      <c r="W4" s="549" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="547"/>
+      <c r="X4" s="549"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -31398,8 +31470,8 @@
       <c r="S5" s="324" t="s">
         <v>213</v>
       </c>
-      <c r="W5" s="547"/>
-      <c r="X5" s="547"/>
+      <c r="W5" s="549"/>
+      <c r="X5" s="549"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -32156,7 +32228,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="551">
+      <c r="W19" s="553">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -32208,7 +32280,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="552"/>
+      <c r="W20" s="554"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -32257,8 +32329,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="553"/>
-      <c r="X21" s="553"/>
+      <c r="W21" s="555"/>
+      <c r="X21" s="555"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -32359,8 +32431,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="554"/>
-      <c r="X23" s="554"/>
+      <c r="W23" s="556"/>
+      <c r="X23" s="556"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -32411,8 +32483,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="554"/>
-      <c r="X24" s="554"/>
+      <c r="W24" s="556"/>
+      <c r="X24" s="556"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -32458,8 +32530,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="555"/>
-      <c r="X25" s="555"/>
+      <c r="W25" s="557"/>
+      <c r="X25" s="557"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -32507,8 +32579,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="555"/>
-      <c r="X26" s="555"/>
+      <c r="W26" s="557"/>
+      <c r="X26" s="557"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -32568,9 +32640,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="548"/>
-      <c r="X27" s="549"/>
-      <c r="Y27" s="550"/>
+      <c r="W27" s="550"/>
+      <c r="X27" s="551"/>
+      <c r="Y27" s="552"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -32624,9 +32696,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="549"/>
-      <c r="X28" s="549"/>
-      <c r="Y28" s="550"/>
+      <c r="W28" s="551"/>
+      <c r="X28" s="551"/>
+      <c r="Y28" s="552"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -32942,11 +33014,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="566">
+      <c r="M36" s="568">
         <f>SUM(M5:M35)</f>
         <v>1077791.3</v>
       </c>
-      <c r="N36" s="568">
+      <c r="N36" s="570">
         <f>SUM(N5:N35)</f>
         <v>936398</v>
       </c>
@@ -32954,7 +33026,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="570">
+      <c r="Q36" s="572">
         <f>SUM(Q5:Q35)</f>
         <v>-14262.940000000002</v>
       </c>
@@ -32973,13 +33045,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="567"/>
-      <c r="N37" s="569"/>
+      <c r="M37" s="569"/>
+      <c r="N37" s="571"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="571"/>
+      <c r="Q37" s="573"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -33253,26 +33325,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="521" t="s">
+      <c r="H52" s="523" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="522"/>
+      <c r="I52" s="524"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="523">
+      <c r="K52" s="525">
         <f>I50+L50</f>
         <v>90750.75</v>
       </c>
-      <c r="L52" s="556"/>
+      <c r="L52" s="558"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="527" t="s">
+      <c r="D53" s="529" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="527"/>
+      <c r="E53" s="529"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>1739855.03</v>
@@ -33281,29 +33353,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="557" t="s">
+      <c r="D54" s="559" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="557"/>
+      <c r="E54" s="559"/>
       <c r="F54" s="111">
         <v>-1567070.66</v>
       </c>
-      <c r="I54" s="528" t="s">
+      <c r="I54" s="530" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="529"/>
-      <c r="K54" s="530">
+      <c r="J54" s="531"/>
+      <c r="K54" s="532">
         <f>F56+F57+F58</f>
         <v>703192.8600000001</v>
       </c>
-      <c r="L54" s="530"/>
-      <c r="M54" s="558" t="s">
+      <c r="L54" s="532"/>
+      <c r="M54" s="560" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="559"/>
-      <c r="O54" s="559"/>
-      <c r="P54" s="559"/>
-      <c r="Q54" s="560"/>
+      <c r="N54" s="561"/>
+      <c r="O54" s="561"/>
+      <c r="P54" s="561"/>
+      <c r="Q54" s="562"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="313" t="s">
@@ -33317,11 +33389,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="561"/>
-      <c r="N55" s="562"/>
-      <c r="O55" s="562"/>
-      <c r="P55" s="562"/>
-      <c r="Q55" s="563"/>
+      <c r="M55" s="563"/>
+      <c r="N55" s="564"/>
+      <c r="O55" s="564"/>
+      <c r="P55" s="564"/>
+      <c r="Q55" s="565"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -33339,11 +33411,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="532">
+      <c r="K56" s="534">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="533"/>
+      <c r="L56" s="535"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -33360,22 +33432,22 @@
       <c r="C58" s="112">
         <v>44563</v>
       </c>
-      <c r="D58" s="510" t="s">
+      <c r="D58" s="512" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="511"/>
+      <c r="E58" s="513"/>
       <c r="F58" s="113">
         <v>754143.23</v>
       </c>
-      <c r="I58" s="512" t="s">
+      <c r="I58" s="514" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="513"/>
-      <c r="K58" s="514">
+      <c r="J58" s="515"/>
+      <c r="K58" s="516">
         <f>K54+K56</f>
         <v>135803.51000000013</v>
       </c>
-      <c r="L58" s="514"/>
+      <c r="L58" s="516"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -35938,7 +36010,7 @@
       <c r="C75" s="214"/>
       <c r="D75" s="256"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="572" t="s">
+      <c r="F75" s="574" t="s">
         <v>207</v>
       </c>
       <c r="K75" s="1"/>
@@ -35951,7 +36023,7 @@
       <c r="C76" s="1"/>
       <c r="D76" s="256"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="573"/>
+      <c r="F76" s="575"/>
       <c r="K76" s="1"/>
       <c r="L76" s="256"/>
       <c r="M76" s="3"/>
@@ -36243,23 +36315,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="534"/>
-      <c r="C1" s="576" t="s">
+      <c r="B1" s="536"/>
+      <c r="C1" s="578" t="s">
         <v>316</v>
       </c>
-      <c r="D1" s="577"/>
-      <c r="E1" s="577"/>
-      <c r="F1" s="577"/>
-      <c r="G1" s="577"/>
-      <c r="H1" s="577"/>
-      <c r="I1" s="577"/>
-      <c r="J1" s="577"/>
-      <c r="K1" s="577"/>
-      <c r="L1" s="577"/>
-      <c r="M1" s="577"/>
+      <c r="D1" s="579"/>
+      <c r="E1" s="579"/>
+      <c r="F1" s="579"/>
+      <c r="G1" s="579"/>
+      <c r="H1" s="579"/>
+      <c r="I1" s="579"/>
+      <c r="J1" s="579"/>
+      <c r="K1" s="579"/>
+      <c r="L1" s="579"/>
+      <c r="M1" s="579"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="535"/>
+      <c r="B2" s="537"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -36269,24 +36341,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="538" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="539"/>
+      <c r="B3" s="540" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="541"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="540" t="s">
+      <c r="H3" s="542" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="540"/>
+      <c r="I3" s="542"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="564" t="s">
+      <c r="P3" s="566" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="574" t="s">
+      <c r="R3" s="576" t="s">
         <v>216</v>
       </c>
     </row>
@@ -36301,14 +36373,14 @@
       <c r="D4" s="18">
         <v>44563</v>
       </c>
-      <c r="E4" s="541" t="s">
+      <c r="E4" s="543" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="542"/>
-      <c r="H4" s="543" t="s">
+      <c r="F4" s="544"/>
+      <c r="H4" s="545" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="544"/>
+      <c r="I4" s="546"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -36318,15 +36390,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="565"/>
+      <c r="P4" s="567"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="575"/>
-      <c r="W4" s="547" t="s">
+      <c r="R4" s="577"/>
+      <c r="W4" s="549" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="547"/>
+      <c r="X4" s="549"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -36377,8 +36449,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="547"/>
-      <c r="X5" s="547"/>
+      <c r="W5" s="549"/>
+      <c r="X5" s="549"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -37142,7 +37214,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="551">
+      <c r="W19" s="553">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -37195,7 +37267,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="552"/>
+      <c r="W20" s="554"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -37244,8 +37316,8 @@
         <v>377273.87</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="553"/>
-      <c r="X21" s="553"/>
+      <c r="W21" s="555"/>
+      <c r="X21" s="555"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -37345,8 +37417,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="554"/>
-      <c r="X23" s="554"/>
+      <c r="W23" s="556"/>
+      <c r="X23" s="556"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -37401,8 +37473,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="554"/>
-      <c r="X24" s="554"/>
+      <c r="W24" s="556"/>
+      <c r="X24" s="556"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -37447,8 +37519,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="555"/>
-      <c r="X25" s="555"/>
+      <c r="W25" s="557"/>
+      <c r="X25" s="557"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -37496,8 +37568,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="555"/>
-      <c r="X26" s="555"/>
+      <c r="W26" s="557"/>
+      <c r="X26" s="557"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -37551,9 +37623,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="548"/>
-      <c r="X27" s="549"/>
-      <c r="Y27" s="550"/>
+      <c r="W27" s="550"/>
+      <c r="X27" s="551"/>
+      <c r="Y27" s="552"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -37607,9 +37679,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="549"/>
-      <c r="X28" s="549"/>
-      <c r="Y28" s="550"/>
+      <c r="W28" s="551"/>
+      <c r="X28" s="551"/>
+      <c r="Y28" s="552"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -37920,11 +37992,11 @@
       <c r="L36" s="44">
         <v>13275.84</v>
       </c>
-      <c r="M36" s="566">
+      <c r="M36" s="568">
         <f>SUM(M5:M35)</f>
         <v>1818445.73</v>
       </c>
-      <c r="N36" s="568">
+      <c r="N36" s="570">
         <f>SUM(N5:N35)</f>
         <v>739014</v>
       </c>
@@ -37932,7 +38004,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="570">
+      <c r="Q36" s="572">
         <f>SUM(Q5:Q35)</f>
         <v>-7.2800000000133878</v>
       </c>
@@ -37957,13 +38029,13 @@
       <c r="L37" s="61">
         <v>15060.32</v>
       </c>
-      <c r="M37" s="567"/>
-      <c r="N37" s="569"/>
+      <c r="M37" s="569"/>
+      <c r="N37" s="571"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="571"/>
+      <c r="Q37" s="573"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -38256,26 +38328,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="521" t="s">
+      <c r="H52" s="523" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="522"/>
+      <c r="I52" s="524"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="523">
+      <c r="K52" s="525">
         <f>I50+L50</f>
         <v>158798.12</v>
       </c>
-      <c r="L52" s="556"/>
+      <c r="L52" s="558"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="527" t="s">
+      <c r="D53" s="529" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="527"/>
+      <c r="E53" s="529"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>2078470.75</v>
@@ -38284,22 +38356,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="557" t="s">
+      <c r="D54" s="559" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="557"/>
+      <c r="E54" s="559"/>
       <c r="F54" s="111">
         <v>-1448401.2</v>
       </c>
-      <c r="I54" s="528" t="s">
+      <c r="I54" s="530" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="529"/>
-      <c r="K54" s="530">
+      <c r="J54" s="531"/>
+      <c r="K54" s="532">
         <f>F56+F57+F58</f>
         <v>1025960.7</v>
       </c>
-      <c r="L54" s="530"/>
+      <c r="L54" s="532"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -38340,11 +38412,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="532">
+      <c r="K56" s="534">
         <f>-C4</f>
         <v>-754143.23</v>
       </c>
-      <c r="L56" s="533"/>
+      <c r="L56" s="535"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -38361,22 +38433,22 @@
       <c r="C58" s="112">
         <v>44591</v>
       </c>
-      <c r="D58" s="510" t="s">
+      <c r="D58" s="512" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="511"/>
+      <c r="E58" s="513"/>
       <c r="F58" s="113">
         <v>1149740.4099999999</v>
       </c>
-      <c r="I58" s="512" t="s">
+      <c r="I58" s="514" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="513"/>
-      <c r="K58" s="514">
+      <c r="J58" s="515"/>
+      <c r="K58" s="516">
         <f>K54+K56</f>
         <v>271817.46999999997</v>
       </c>
-      <c r="L58" s="514"/>
+      <c r="L58" s="516"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -40245,12 +40317,12 @@
     </row>
     <row r="43" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="245"/>
-      <c r="B43" s="578" t="s">
+      <c r="B43" s="580" t="s">
         <v>413</v>
       </c>
-      <c r="C43" s="579"/>
-      <c r="D43" s="579"/>
-      <c r="E43" s="580"/>
+      <c r="C43" s="581"/>
+      <c r="D43" s="581"/>
+      <c r="E43" s="582"/>
       <c r="F43" s="392">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -40278,10 +40350,10 @@
     </row>
     <row r="44" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="245"/>
-      <c r="B44" s="581"/>
-      <c r="C44" s="582"/>
-      <c r="D44" s="582"/>
-      <c r="E44" s="583"/>
+      <c r="B44" s="583"/>
+      <c r="C44" s="584"/>
+      <c r="D44" s="584"/>
+      <c r="E44" s="585"/>
       <c r="F44" s="392">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -40309,10 +40381,10 @@
     </row>
     <row r="45" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="245"/>
-      <c r="B45" s="584"/>
-      <c r="C45" s="585"/>
-      <c r="D45" s="585"/>
-      <c r="E45" s="586"/>
+      <c r="B45" s="586"/>
+      <c r="C45" s="587"/>
+      <c r="D45" s="587"/>
+      <c r="E45" s="588"/>
       <c r="F45" s="392">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -40355,10 +40427,10 @@
     </row>
     <row r="47" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="245"/>
-      <c r="B47" s="593" t="s">
+      <c r="B47" s="595" t="s">
         <v>593</v>
       </c>
-      <c r="C47" s="594"/>
+      <c r="C47" s="596"/>
       <c r="D47" s="253"/>
       <c r="E47" s="69"/>
       <c r="F47" s="137">
@@ -40380,8 +40452,8 @@
     </row>
     <row r="48" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="245"/>
-      <c r="B48" s="595"/>
-      <c r="C48" s="596"/>
+      <c r="B48" s="597"/>
+      <c r="C48" s="598"/>
       <c r="D48" s="253"/>
       <c r="E48" s="69"/>
       <c r="F48" s="137">
@@ -40389,11 +40461,11 @@
         <v>0</v>
       </c>
       <c r="I48" s="348"/>
-      <c r="J48" s="587" t="s">
+      <c r="J48" s="589" t="s">
         <v>414</v>
       </c>
-      <c r="K48" s="588"/>
-      <c r="L48" s="589"/>
+      <c r="K48" s="590"/>
+      <c r="L48" s="591"/>
       <c r="M48" s="206"/>
       <c r="N48" s="137">
         <f>N47+K48-M48</f>
@@ -40411,9 +40483,9 @@
         <v>0</v>
       </c>
       <c r="I49" s="348"/>
-      <c r="J49" s="590"/>
-      <c r="K49" s="591"/>
-      <c r="L49" s="592"/>
+      <c r="J49" s="592"/>
+      <c r="K49" s="593"/>
+      <c r="L49" s="594"/>
       <c r="M49" s="206"/>
       <c r="N49" s="137">
         <f t="shared" si="1"/>
@@ -40430,10 +40502,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I50" s="597" t="s">
+      <c r="I50" s="599" t="s">
         <v>594</v>
       </c>
-      <c r="J50" s="598"/>
+      <c r="J50" s="600"/>
       <c r="K50" s="215">
         <v>0</v>
       </c>
@@ -40454,8 +40526,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I51" s="597"/>
-      <c r="J51" s="598"/>
+      <c r="I51" s="599"/>
+      <c r="J51" s="600"/>
       <c r="K51" s="69"/>
       <c r="L51" s="253"/>
       <c r="M51" s="69"/>
@@ -40474,8 +40546,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I52" s="597"/>
-      <c r="J52" s="598"/>
+      <c r="I52" s="599"/>
+      <c r="J52" s="600"/>
       <c r="K52" s="69"/>
       <c r="L52" s="253"/>
       <c r="M52" s="69"/>
@@ -40494,8 +40566,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I53" s="597"/>
-      <c r="J53" s="598"/>
+      <c r="I53" s="599"/>
+      <c r="J53" s="600"/>
       <c r="K53" s="69"/>
       <c r="L53" s="253"/>
       <c r="M53" s="69"/>
@@ -40514,8 +40586,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I54" s="597"/>
-      <c r="J54" s="598"/>
+      <c r="I54" s="599"/>
+      <c r="J54" s="600"/>
       <c r="K54" s="69"/>
       <c r="L54" s="253"/>
       <c r="M54" s="69"/>
@@ -40534,8 +40606,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I55" s="597"/>
-      <c r="J55" s="598"/>
+      <c r="I55" s="599"/>
+      <c r="J55" s="600"/>
       <c r="K55" s="69"/>
       <c r="L55" s="253"/>
       <c r="M55" s="69"/>
@@ -40554,8 +40626,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I56" s="597"/>
-      <c r="J56" s="598"/>
+      <c r="I56" s="599"/>
+      <c r="J56" s="600"/>
       <c r="K56" s="69"/>
       <c r="L56" s="253"/>
       <c r="M56" s="69"/>
@@ -40574,8 +40646,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I57" s="597"/>
-      <c r="J57" s="598"/>
+      <c r="I57" s="599"/>
+      <c r="J57" s="600"/>
       <c r="K57" s="69"/>
       <c r="L57" s="253"/>
       <c r="M57" s="69"/>
@@ -40594,8 +40666,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I58" s="597"/>
-      <c r="J58" s="598"/>
+      <c r="I58" s="599"/>
+      <c r="J58" s="600"/>
       <c r="K58" s="69"/>
       <c r="L58" s="253"/>
       <c r="M58" s="69"/>
@@ -40614,8 +40686,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I59" s="597"/>
-      <c r="J59" s="598"/>
+      <c r="I59" s="599"/>
+      <c r="J59" s="600"/>
       <c r="K59" s="69"/>
       <c r="L59" s="253"/>
       <c r="M59" s="69"/>
@@ -40634,8 +40706,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I60" s="597"/>
-      <c r="J60" s="598"/>
+      <c r="I60" s="599"/>
+      <c r="J60" s="600"/>
       <c r="K60" s="69"/>
       <c r="L60" s="253"/>
       <c r="M60" s="69"/>
@@ -40654,8 +40726,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I61" s="597"/>
-      <c r="J61" s="598"/>
+      <c r="I61" s="599"/>
+      <c r="J61" s="600"/>
       <c r="K61" s="69"/>
       <c r="L61" s="253"/>
       <c r="M61" s="69"/>
@@ -40674,8 +40746,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I62" s="597"/>
-      <c r="J62" s="598"/>
+      <c r="I62" s="599"/>
+      <c r="J62" s="600"/>
       <c r="K62" s="34"/>
       <c r="L62" s="118"/>
       <c r="M62" s="34"/>
@@ -40694,8 +40766,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I63" s="597"/>
-      <c r="J63" s="598"/>
+      <c r="I63" s="599"/>
+      <c r="J63" s="600"/>
       <c r="K63" s="34"/>
       <c r="L63" s="118"/>
       <c r="M63" s="34"/>
@@ -40714,8 +40786,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I64" s="597"/>
-      <c r="J64" s="598"/>
+      <c r="I64" s="599"/>
+      <c r="J64" s="600"/>
       <c r="K64" s="34"/>
       <c r="L64" s="118"/>
       <c r="M64" s="34"/>
@@ -40734,8 +40806,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I65" s="597"/>
-      <c r="J65" s="598"/>
+      <c r="I65" s="599"/>
+      <c r="J65" s="600"/>
       <c r="K65" s="34"/>
       <c r="L65" s="118"/>
       <c r="M65" s="34"/>
@@ -40754,8 +40826,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I66" s="597"/>
-      <c r="J66" s="598"/>
+      <c r="I66" s="599"/>
+      <c r="J66" s="600"/>
       <c r="K66" s="34"/>
       <c r="L66" s="118"/>
       <c r="M66" s="34"/>
@@ -40774,8 +40846,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I67" s="597"/>
-      <c r="J67" s="598"/>
+      <c r="I67" s="599"/>
+      <c r="J67" s="600"/>
       <c r="K67" s="34"/>
       <c r="L67" s="118"/>
       <c r="M67" s="34"/>
@@ -40794,8 +40866,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I68" s="597"/>
-      <c r="J68" s="598"/>
+      <c r="I68" s="599"/>
+      <c r="J68" s="600"/>
       <c r="K68" s="69"/>
       <c r="L68" s="254"/>
       <c r="M68" s="69"/>
@@ -40814,8 +40886,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I69" s="597"/>
-      <c r="J69" s="598"/>
+      <c r="I69" s="599"/>
+      <c r="J69" s="600"/>
       <c r="K69" s="69"/>
       <c r="L69" s="254"/>
       <c r="M69" s="69"/>
@@ -40834,8 +40906,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I70" s="597"/>
-      <c r="J70" s="598"/>
+      <c r="I70" s="599"/>
+      <c r="J70" s="600"/>
       <c r="K70" s="69"/>
       <c r="L70" s="254"/>
       <c r="M70" s="69"/>
@@ -40854,8 +40926,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I71" s="597"/>
-      <c r="J71" s="598"/>
+      <c r="I71" s="599"/>
+      <c r="J71" s="600"/>
       <c r="K71" s="69"/>
       <c r="L71" s="254"/>
       <c r="M71" s="69"/>
@@ -40874,8 +40946,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I72" s="597"/>
-      <c r="J72" s="598"/>
+      <c r="I72" s="599"/>
+      <c r="J72" s="600"/>
       <c r="K72" s="69"/>
       <c r="L72" s="254"/>
       <c r="M72" s="69"/>
@@ -40894,8 +40966,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I73" s="597"/>
-      <c r="J73" s="598"/>
+      <c r="I73" s="599"/>
+      <c r="J73" s="600"/>
       <c r="K73" s="69"/>
       <c r="L73" s="254"/>
       <c r="M73" s="69"/>
@@ -40914,8 +40986,8 @@
         <f>F73+C74-E74</f>
         <v>0</v>
       </c>
-      <c r="I74" s="597"/>
-      <c r="J74" s="598"/>
+      <c r="I74" s="599"/>
+      <c r="J74" s="600"/>
       <c r="K74" s="69"/>
       <c r="L74" s="254"/>
       <c r="M74" s="69"/>
@@ -40934,8 +41006,8 @@
         <f>F74+C75-E75</f>
         <v>0</v>
       </c>
-      <c r="I75" s="597"/>
-      <c r="J75" s="598"/>
+      <c r="I75" s="599"/>
+      <c r="J75" s="600"/>
       <c r="K75" s="69"/>
       <c r="L75" s="254"/>
       <c r="M75" s="69"/>
@@ -40954,8 +41026,8 @@
         <f>F75+C76-E76</f>
         <v>0</v>
       </c>
-      <c r="I76" s="597"/>
-      <c r="J76" s="598"/>
+      <c r="I76" s="599"/>
+      <c r="J76" s="600"/>
       <c r="K76" s="69"/>
       <c r="L76" s="254"/>
       <c r="M76" s="69"/>
@@ -40974,8 +41046,8 @@
         <f>F76+C77-E77</f>
         <v>0</v>
       </c>
-      <c r="I77" s="597"/>
-      <c r="J77" s="598"/>
+      <c r="I77" s="599"/>
+      <c r="J77" s="600"/>
       <c r="K77" s="69"/>
       <c r="L77" s="254"/>
       <c r="M77" s="69"/>
@@ -40996,8 +41068,8 @@
         <f>F77+C78-E78</f>
         <v>0</v>
       </c>
-      <c r="I78" s="599"/>
-      <c r="J78" s="600"/>
+      <c r="I78" s="601"/>
+      <c r="J78" s="602"/>
       <c r="K78" s="151">
         <v>0</v>
       </c>
@@ -41042,7 +41114,7 @@
       <c r="C80" s="214"/>
       <c r="D80" s="256"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="572" t="s">
+      <c r="F80" s="574" t="s">
         <v>207</v>
       </c>
       <c r="K80" s="1"/>
@@ -41054,7 +41126,7 @@
       <c r="C81" s="1"/>
       <c r="D81" s="256"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="573"/>
+      <c r="F81" s="575"/>
       <c r="K81" s="1"/>
       <c r="M81" s="3"/>
       <c r="N81" s="1"/>
@@ -41342,23 +41414,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="534"/>
-      <c r="C1" s="576" t="s">
+      <c r="B1" s="536"/>
+      <c r="C1" s="578" t="s">
         <v>646</v>
       </c>
-      <c r="D1" s="577"/>
-      <c r="E1" s="577"/>
-      <c r="F1" s="577"/>
-      <c r="G1" s="577"/>
-      <c r="H1" s="577"/>
-      <c r="I1" s="577"/>
-      <c r="J1" s="577"/>
-      <c r="K1" s="577"/>
-      <c r="L1" s="577"/>
-      <c r="M1" s="577"/>
+      <c r="D1" s="579"/>
+      <c r="E1" s="579"/>
+      <c r="F1" s="579"/>
+      <c r="G1" s="579"/>
+      <c r="H1" s="579"/>
+      <c r="I1" s="579"/>
+      <c r="J1" s="579"/>
+      <c r="K1" s="579"/>
+      <c r="L1" s="579"/>
+      <c r="M1" s="579"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="535"/>
+      <c r="B2" s="537"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -41368,24 +41440,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="538" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="539"/>
+      <c r="B3" s="540" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="541"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="540" t="s">
+      <c r="H3" s="542" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="540"/>
+      <c r="I3" s="542"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="564" t="s">
+      <c r="P3" s="566" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="574" t="s">
+      <c r="R3" s="576" t="s">
         <v>216</v>
       </c>
     </row>
@@ -41400,14 +41472,14 @@
       <c r="D4" s="18">
         <v>44591</v>
       </c>
-      <c r="E4" s="541" t="s">
+      <c r="E4" s="543" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="542"/>
-      <c r="H4" s="543" t="s">
+      <c r="F4" s="544"/>
+      <c r="H4" s="545" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="544"/>
+      <c r="I4" s="546"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -41417,15 +41489,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="565"/>
+      <c r="P4" s="567"/>
       <c r="Q4" s="322" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="575"/>
-      <c r="W4" s="547" t="s">
+      <c r="R4" s="577"/>
+      <c r="W4" s="549" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="547"/>
+      <c r="X4" s="549"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -41476,8 +41548,8 @@
         <v>0</v>
       </c>
       <c r="S5" s="324"/>
-      <c r="W5" s="547"/>
-      <c r="X5" s="547"/>
+      <c r="W5" s="549"/>
+      <c r="X5" s="549"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -42238,7 +42310,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="551">
+      <c r="W19" s="553">
         <f>SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -42290,7 +42362,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="552"/>
+      <c r="W20" s="554"/>
       <c r="X20" s="268"/>
       <c r="Y20" s="233"/>
     </row>
@@ -42339,8 +42411,8 @@
         <v>18072</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="553"/>
-      <c r="X21" s="553"/>
+      <c r="W21" s="555"/>
+      <c r="X21" s="555"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -42439,8 +42511,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="554"/>
-      <c r="X23" s="554"/>
+      <c r="W23" s="556"/>
+      <c r="X23" s="556"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -42495,8 +42567,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="554"/>
-      <c r="X24" s="554"/>
+      <c r="W24" s="556"/>
+      <c r="X24" s="556"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -42544,8 +42616,8 @@
       <c r="R25" s="319">
         <v>0</v>
       </c>
-      <c r="W25" s="555"/>
-      <c r="X25" s="555"/>
+      <c r="W25" s="557"/>
+      <c r="X25" s="557"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -42593,8 +42665,8 @@
       <c r="R26" s="319">
         <v>0</v>
       </c>
-      <c r="W26" s="555"/>
-      <c r="X26" s="555"/>
+      <c r="W26" s="557"/>
+      <c r="X26" s="557"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -42642,9 +42714,9 @@
       <c r="R27" s="319">
         <v>0</v>
       </c>
-      <c r="W27" s="548"/>
-      <c r="X27" s="549"/>
-      <c r="Y27" s="550"/>
+      <c r="W27" s="550"/>
+      <c r="X27" s="551"/>
+      <c r="Y27" s="552"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -42692,9 +42764,9 @@
       <c r="R28" s="319">
         <v>0</v>
       </c>
-      <c r="W28" s="549"/>
-      <c r="X28" s="549"/>
-      <c r="Y28" s="550"/>
+      <c r="W28" s="551"/>
+      <c r="X28" s="551"/>
+      <c r="Y28" s="552"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -43035,11 +43107,11 @@
       <c r="J36" s="266"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="566">
+      <c r="M36" s="568">
         <f>SUM(M5:M35)</f>
         <v>2143864.4900000002</v>
       </c>
-      <c r="N36" s="568">
+      <c r="N36" s="570">
         <f>SUM(N5:N35)</f>
         <v>791108</v>
       </c>
@@ -43047,7 +43119,7 @@
       <c r="P36" s="277">
         <v>0</v>
       </c>
-      <c r="Q36" s="601">
+      <c r="Q36" s="603">
         <f>SUM(Q5:Q35)</f>
         <v>111.43999999999505</v>
       </c>
@@ -43072,13 +43144,13 @@
       <c r="L37" s="61">
         <v>16518.78</v>
       </c>
-      <c r="M37" s="567"/>
-      <c r="N37" s="569"/>
+      <c r="M37" s="569"/>
+      <c r="N37" s="571"/>
       <c r="O37" s="276"/>
       <c r="P37" s="277">
         <v>0</v>
       </c>
-      <c r="Q37" s="602"/>
+      <c r="Q37" s="604"/>
       <c r="R37" s="227" t="s">
         <v>7</v>
       </c>
@@ -43128,11 +43200,11 @@
       <c r="L39" s="61">
         <v>14981.03</v>
       </c>
-      <c r="M39" s="603">
+      <c r="M39" s="605">
         <f>M36+N36</f>
         <v>2934972.49</v>
       </c>
-      <c r="N39" s="604"/>
+      <c r="N39" s="606"/>
       <c r="P39" s="34">
         <f>SUM(P5:P38)</f>
         <v>3450079.65</v>
@@ -43380,26 +43452,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="521" t="s">
+      <c r="H52" s="523" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="522"/>
+      <c r="I52" s="524"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="523">
+      <c r="K52" s="525">
         <f>I50+L50</f>
         <v>197471.8</v>
       </c>
-      <c r="L52" s="556"/>
+      <c r="L52" s="558"/>
       <c r="M52" s="272"/>
       <c r="N52" s="272"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="527" t="s">
+      <c r="D53" s="529" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="527"/>
+      <c r="E53" s="529"/>
       <c r="F53" s="312">
         <f>F50-K52-C50</f>
         <v>2057786.11</v>
@@ -43408,22 +43480,22 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="557" t="s">
+      <c r="D54" s="559" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="557"/>
+      <c r="E54" s="559"/>
       <c r="F54" s="111">
         <v>-1702928.14</v>
       </c>
-      <c r="I54" s="528" t="s">
+      <c r="I54" s="530" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="529"/>
-      <c r="K54" s="530">
+      <c r="J54" s="531"/>
+      <c r="K54" s="532">
         <f>F56+F57+F58</f>
         <v>1147965.3400000003</v>
       </c>
-      <c r="L54" s="530"/>
+      <c r="L54" s="532"/>
       <c r="M54" s="404"/>
       <c r="N54" s="404"/>
       <c r="O54" s="404"/>
@@ -43464,11 +43536,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="532">
+      <c r="K56" s="534">
         <f>-C4</f>
         <v>-1149740.4099999999</v>
       </c>
-      <c r="L56" s="533"/>
+      <c r="L56" s="535"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -43485,22 +43557,22 @@
       <c r="C58" s="112">
         <v>44619</v>
       </c>
-      <c r="D58" s="510" t="s">
+      <c r="D58" s="512" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="511"/>
+      <c r="E58" s="513"/>
       <c r="F58" s="113">
         <v>1266568.45</v>
       </c>
-      <c r="I58" s="512" t="s">
+      <c r="I58" s="514" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="513"/>
-      <c r="K58" s="514">
+      <c r="J58" s="515"/>
+      <c r="K58" s="516">
         <f>K54+K56</f>
         <v>-1775.0699999995995</v>
       </c>
-      <c r="L58" s="514"/>
+      <c r="L58" s="516"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>

</xml_diff>